<commit_message>
📊 Horarios actualizados Línea 141 - 938
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:20:29</t>
+          <t>Última actualización: 01:34:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 2</t>
         </is>
       </c>
     </row>
@@ -478,23 +478,48 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00:20:29</t>
+          <t>01:34:47</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01:25</t>
+          <t>03:01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>01:34:47</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>03:02</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>88</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -529,7 +554,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:20:29</t>
+          <t>Última actualización: 01:34:47</t>
         </is>
       </c>
     </row>
@@ -569,7 +594,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:20:29</t>
+          <t>Última actualización: 01:34:47</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 939
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:34:47</t>
+          <t>Última actualización: 02:06:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -478,12 +478,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:34:47</t>
+          <t>02:06:16</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:01</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,23 +503,48 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:34:47</t>
+          <t>02:06:16</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>02:06:16</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>04:02</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>116</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -554,7 +579,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:34:47</t>
+          <t>Última actualización: 02:06:16</t>
         </is>
       </c>
     </row>
@@ -594,7 +619,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:34:47</t>
+          <t>Última actualización: 02:06:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 940
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -437,7 +437,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:06:16</t>
+          <t>Última actualización: 02:38:37</t>
         </is>
       </c>
     </row>
@@ -478,7 +478,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:06:16</t>
+          <t>02:38:37</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,7 +503,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:06:16</t>
+          <t>02:38:37</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,12 +528,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:06:16</t>
+          <t>02:38:37</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:02</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -579,7 +579,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:06:16</t>
+          <t>Última actualización: 02:38:37</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:06:16</t>
+          <t>Última actualización: 02:38:37</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 941
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:38:37</t>
+          <t>Última actualización: 02:54:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -478,7 +478,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:38:37</t>
+          <t>02:54:27</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,7 +503,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:38:37</t>
+          <t>02:54:27</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,7 +528,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:38:37</t>
+          <t>02:54:27</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -542,9 +542,59 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>02:54:27</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>04:46</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>112</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>02:54:27</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>119</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -561,7 +611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,14 +629,66 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:38:37</t>
+          <t>Última actualización: 02:54:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 0</t>
+          <t>Total filas: 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>02:54:27</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>04:46</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>112</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -619,7 +721,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:38:37</t>
+          <t>Última actualización: 02:54:27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 942
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -437,7 +437,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:54:27</t>
+          <t>Última actualización: 03:19:42</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:54:27</t>
+          <t>03:19:42</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:54:27</t>
+          <t>03:19:42</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:54:27</t>
+          <t>03:19:42</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,21 +553,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02:54:27</t>
+          <t>03:19:42</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>02:54:27</t>
+          <t>03:19:42</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:11</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -629,7 +629,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:54:27</t>
+          <t>Última actualización: 03:19:42</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:54:27</t>
+          <t>03:19:42</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -684,7 +684,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:54:27</t>
+          <t>Última actualización: 03:19:42</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 943
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:19:42</t>
+          <t>Última actualización: 03:51:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03:19:42</t>
+          <t>03:51:22</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:02</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03:19:42</t>
+          <t>03:51:22</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03:19:42</t>
+          <t>03:51:22</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,21 +553,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03:19:42</t>
+          <t>03:51:22</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:11</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,23 +578,73 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03:19:42</t>
+          <t>03:51:22</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:11</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>03:51:22</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>05:32</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>101</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>03:51:22</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>05:44</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>113</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -629,7 +679,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:19:42</t>
+          <t>Última actualización: 03:51:22</t>
         </is>
       </c>
     </row>
@@ -670,12 +720,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03:19:42</t>
+          <t>03:51:22</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -684,7 +734,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -721,7 +771,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:19:42</t>
+          <t>Última actualización: 03:51:22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 944
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:51:22</t>
+          <t>Última actualización: 04:15:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03:51:22</t>
+          <t>04:15:01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:02</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03:51:22</t>
+          <t>04:15:01</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03:51:22</t>
+          <t>04:15:01</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,21 +553,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03:51:22</t>
+          <t>04:15:01</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:11</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03:51:22</t>
+          <t>04:15:01</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:32</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,21 +603,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03:51:22</t>
+          <t>04:15:01</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,23 +628,98 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03:51:22</t>
+          <t>04:15:01</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>05:52</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>04:15:01</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>06:01</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>106</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>04:15:01</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06:04</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>109</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>04:15:01</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>116</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -661,7 +736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,14 +754,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:51:22</t>
+          <t>Última actualización: 04:15:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 2</t>
         </is>
       </c>
     </row>
@@ -720,7 +795,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03:51:22</t>
+          <t>04:15:01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -734,9 +809,34 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>04:15:01</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>116</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -771,7 +871,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:51:22</t>
+          <t>Última actualización: 04:15:01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 945
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:15:01</t>
+          <t>Última actualización: 04:34:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 14</t>
         </is>
       </c>
     </row>
@@ -478,7 +478,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,7 +503,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,12 +528,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>05:11</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,7 +628,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,7 +653,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,7 +703,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -717,9 +717,109 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>04:34:13</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>06:24</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>110</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>04:34:13</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>113</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>04:34:13</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>06:31</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>117</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>04:34:13</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>06:31</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>117</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -754,7 +854,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:15:01</t>
+          <t>Última actualización: 04:34:13</t>
         </is>
       </c>
     </row>
@@ -795,7 +895,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -809,7 +909,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -820,7 +920,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:15:01</t>
+          <t>04:34:13</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -834,7 +934,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -871,7 +971,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:15:01</t>
+          <t>Última actualización: 04:34:13</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 946
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:34:13</t>
+          <t>Última actualización: 04:46:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 14</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -478,7 +478,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,7 +503,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,12 +528,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>05:11</t>
+          <t>05:12</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,7 +628,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,7 +653,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,7 +703,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,7 +778,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -817,9 +817,34 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>04:46:05</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>06:39</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>113</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -854,7 +879,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:34:13</t>
+          <t>Última actualización: 04:46:05</t>
         </is>
       </c>
     </row>
@@ -895,7 +920,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -909,7 +934,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -920,7 +945,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:34:13</t>
+          <t>04:46:05</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -934,7 +959,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -971,7 +996,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:34:13</t>
+          <t>Última actualización: 04:46:05</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 947
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:46:05</t>
+          <t>Última actualización: 04:53:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:17</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>05:12</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,21 +553,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:32</t>
+          <t>05:47</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,21 +603,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,21 +628,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>06:09</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,21 +653,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>06:16</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,21 +703,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:34</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:24</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,98 +753,23 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:41</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E17" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>04:46:05</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>06:31</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>17X38_ROMERO</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>105</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>04:46:05</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>06:31</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>16_SANTA ANA</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>105</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>04:46:05</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>06:39</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>225_C ROCA-H SUR</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>113</v>
-      </c>
-      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -861,7 +786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -879,14 +804,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:46:05</t>
+          <t>Última actualización: 04:53:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 1</t>
         </is>
       </c>
     </row>
@@ -920,48 +845,23 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:46:05</t>
+          <t>04:53:24</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>06:16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>04:46:05</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>06:11</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>85</v>
-      </c>
-      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -996,7 +896,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:46:05</t>
+          <t>Última actualización: 04:53:24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 948
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:53:24</t>
+          <t>Última actualización: 05:16:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 14</t>
         </is>
       </c>
     </row>
@@ -478,17 +478,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>05:17</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,21 +553,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>05:46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:47</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,21 +603,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>06:09</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,21 +628,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:09</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,21 +653,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:16</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:34</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,21 +703,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:34</t>
+          <t>06:40</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,12 +728,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>06:45</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,23 +753,73 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:41</t>
+          <t>06:56</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>05:16:45</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>06:59</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>103</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>05:16:45</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>119</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -786,7 +836,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -804,14 +854,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:53:24</t>
+          <t>Última actualización: 05:16:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -845,12 +895,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:53:24</t>
+          <t>05:16:45</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:16</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -859,9 +909,59 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05:16:45</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>05:16:45</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>119</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -896,7 +996,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:53:24</t>
+          <t>Última actualización: 05:16:45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 949
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:16:45</t>
+          <t>Última actualización: 05:44:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 14</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -478,17 +478,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:47</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>06:09</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,21 +553,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:46</t>
+          <t>06:16</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,21 +603,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06:09</t>
+          <t>06:34</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,21 +628,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:15</t>
+          <t>06:40</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,21 +653,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:41</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:34</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,21 +703,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:40</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:45</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,21 +753,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,23 +803,98 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>07:22</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>05:44:02</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>07:29</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>105</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>05:44:02</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>111</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>05:44:02</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>113</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -854,7 +929,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:16:45</t>
+          <t>Última actualización: 05:44:02</t>
         </is>
       </c>
     </row>
@@ -895,12 +970,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:15</t>
+          <t>06:16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -909,7 +984,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -920,12 +995,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -934,7 +1009,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -945,12 +1020,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:16:45</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -959,7 +1034,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -978,7 +1053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -996,14 +1071,66 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:16:45</t>
+          <t>Última actualización: 05:44:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 0</t>
+          <t>Total filas: 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05:44:02</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>119</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 950
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:44:02</t>
+          <t>Última actualización: 05:58:04</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -528,7 +528,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,12 +628,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:40</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -658,16 +658,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:41</t>
+          <t>06:40</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:41</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,21 +703,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,21 +753,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07:19</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,21 +803,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>07:22</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -828,21 +828,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>07:22</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -853,21 +853,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -878,23 +878,73 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>97</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>07:37</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>113</v>
-      </c>
-      <c r="E22" t="inlineStr">
+      <c r="D23" t="n">
+        <v>99</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>07:55</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>117</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -929,7 +979,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:44:02</t>
+          <t>Última actualización: 05:58:04</t>
         </is>
       </c>
     </row>
@@ -970,7 +1020,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -984,7 +1034,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -995,7 +1045,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1009,7 +1059,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1020,7 +1070,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1034,7 +1084,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1071,7 +1121,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:44:02</t>
+          <t>Última actualización: 05:58:04</t>
         </is>
       </c>
     </row>
@@ -1112,7 +1162,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1126,7 +1176,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 951
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:58:04</t>
+          <t>Última actualización: 06:19:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 36</t>
         </is>
       </c>
     </row>
@@ -578,12 +578,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:29</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -608,16 +608,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06:34</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,21 +628,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>06:33</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,21 +653,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:40</t>
+          <t>06:34</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:41</t>
+          <t>06:38</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -708,16 +708,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:40</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -758,16 +758,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>06:41</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:19</t>
+          <t>06:56</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -808,16 +808,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -828,21 +828,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>07:22</t>
+          <t>06:58</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -858,16 +858,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -878,21 +878,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -908,16 +908,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,23 +928,448 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>07:18</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>59</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>07:19</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>81</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>07:20</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>61</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>62</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>83</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>07:22</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>84</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>07:29</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>70</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>07:34</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>75</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>97</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>07:36</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>77</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>99</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>84</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>07:54</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>95</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
           <t>07:55</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D37" t="n">
         <v>117</v>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>07:59</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>100</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>101</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>112</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>113</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -961,7 +1386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -979,14 +1404,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:58:04</t>
+          <t>Última actualización: 06:19:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -1045,12 +1470,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:56</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1059,7 +1484,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1075,18 +1500,93 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>59</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>56</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>07:16</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D10" t="n">
         <v>78</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>06:19:59</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>84</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1103,7 +1603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1121,14 +1621,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:58:04</t>
+          <t>Última actualización: 06:19:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 2</t>
         </is>
       </c>
     </row>
@@ -1162,23 +1662,48 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>07:42</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>83</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>07:43</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>105</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 952
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:19:59</t>
+          <t>Última actualización: 06:38:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 36</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,21 +753,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:41</t>
+          <t>06:40</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>06:41</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,12 +803,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:56</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -828,21 +828,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>06:58</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -853,12 +853,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:58</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -867,7 +867,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -878,21 +878,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -903,12 +903,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,21 +928,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>07:18</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,12 +953,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>07:19</t>
+          <t>07:18</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -967,7 +967,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -978,21 +978,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>07:20</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1008,16 +1008,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:20</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1053,12 +1053,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>07:22</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1067,7 +1067,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1078,21 +1078,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>07:22</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1103,21 +1103,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>07:34</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1128,12 +1128,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:34</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1153,21 +1153,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,12 +1178,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1203,21 +1203,21 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,21 +1228,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>07:54</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1253,12 +1253,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>07:55</t>
+          <t>07:54</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1278,21 +1278,21 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>05:58:04</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>07:59</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1308,16 +1308,16 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1328,21 +1328,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>08:11</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1353,23 +1353,173 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>82</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>08:06</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>88</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>93</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>06:19:59</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>08:12</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="D44" t="n">
         <v>113</v>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>08:13</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>95</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>08:28</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>110</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>111</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1404,7 +1554,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:19:59</t>
+          <t>Última actualización: 06:38:54</t>
         </is>
       </c>
     </row>
@@ -1470,7 +1620,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1484,7 +1634,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1520,7 +1670,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1534,7 +1684,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1570,7 +1720,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1584,7 +1734,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1603,7 +1753,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1621,14 +1771,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:19:59</t>
+          <t>Última actualización: 06:38:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -1662,7 +1812,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1676,7 +1826,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1704,6 +1854,31 @@
         <v>105</v>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>117</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 953
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:38:54</t>
+          <t>Última actualización: 06:49:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 47</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -828,7 +828,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -978,7 +978,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1103,7 +1103,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1253,21 +1253,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>07:54</t>
+          <t>07:44</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1278,12 +1278,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>07:55</t>
+          <t>07:54</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,21 +1303,21 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>07:59</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1328,12 +1328,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1378,21 +1378,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>08:06</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1403,21 +1403,21 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>08:11</t>
+          <t>08:01</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,21 +1428,21 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>08:06</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,21 +1453,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>08:13</t>
+          <t>08:11</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,21 +1478,21 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>06:19:59</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>08:28</t>
+          <t>08:12</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1503,23 +1503,148 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>06:49:22</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>08:13</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>84</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>06:38:54</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>08:28</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>110</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>06:49:22</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>08:29</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D47" t="n">
-        <v>111</v>
-      </c>
-      <c r="E47" t="inlineStr">
+      <c r="D49" t="n">
+        <v>100</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>06:49:22</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>100</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>06:49:22</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>08:41</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>112</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>06:49:22</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>115</v>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1536,7 +1661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1554,14 +1679,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:38:54</t>
+          <t>Última actualización: 06:49:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -1645,7 +1770,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1659,7 +1784,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1695,7 +1820,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1709,7 +1834,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1737,6 +1862,56 @@
         <v>65</v>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06:49:22</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:44</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>55</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>06:49:22</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>115</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1753,7 +1928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1771,14 +1946,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:38:54</t>
+          <t>Última actualización: 06:49:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -1837,7 +2012,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:49:22</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1851,7 +2026,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1879,6 +2054,31 @@
         <v>117</v>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>06:49:22</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>08:36</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>107</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 954
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:49:22</t>
+          <t>Última actualización: 06:56:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 47</t>
+          <t>Total filas: 49</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -828,7 +828,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -978,7 +978,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1078,7 +1078,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1103,7 +1103,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1253,7 +1253,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1503,7 +1503,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1553,7 +1553,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1578,7 +1578,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1603,7 +1603,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1642,9 +1642,59 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>08:52</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>116</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>117</v>
+      </c>
+      <c r="E54" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1661,7 +1711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1679,14 +1729,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:49:22</t>
+          <t>Última actualización: 06:56:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -1770,7 +1820,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1784,7 +1834,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1820,7 +1870,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1834,7 +1884,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1870,7 +1920,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1884,7 +1934,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1895,7 +1945,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1909,9 +1959,34 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>117</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1928,7 +2003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1946,14 +2021,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:49:22</t>
+          <t>Última actualización: 06:56:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -2012,7 +2087,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2026,7 +2101,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -2062,7 +2137,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2076,11 +2151,36 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>08:51</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>115</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 955
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:56:24</t>
+          <t>Última actualización: 07:15:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 49</t>
+          <t>Total filas: 52</t>
         </is>
       </c>
     </row>
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -978,7 +978,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06:19:59</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1103,7 +1103,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1503,7 +1503,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1553,7 +1553,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1578,7 +1578,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1603,7 +1603,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,12 +1628,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1658,16 +1658,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,23 +1678,98 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>08:51</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>96</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>06:56:24</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>08:52</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>116</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
         <is>
           <t>08:53</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D54" t="n">
-        <v>117</v>
-      </c>
-      <c r="E54" t="inlineStr">
+      <c r="D56" t="n">
+        <v>98</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>102</v>
+      </c>
+      <c r="E57" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1711,7 +1786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1729,14 +1804,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:56:24</t>
+          <t>Última actualización: 07:15:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
     </row>
@@ -1845,7 +1920,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1859,7 +1934,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1895,7 +1970,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1909,7 +1984,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1945,12 +2020,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1959,7 +2034,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1975,18 +2050,68 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>108</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>08:53</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>117</v>
-      </c>
-      <c r="E14" t="inlineStr">
+      <c r="D15" t="n">
+        <v>98</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>102</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2003,7 +2128,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2021,14 +2146,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:56:24</t>
+          <t>Última actualización: 07:15:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -2062,7 +2187,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2076,7 +2201,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -2112,7 +2237,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2126,7 +2251,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2162,23 +2287,48 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>08:50</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>95</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>06:56:24</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>08:51</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>115</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 956
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:15:48</t>
+          <t>Última actualización: 07:40:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 52</t>
+          <t>Total filas: 60</t>
         </is>
       </c>
     </row>
@@ -1253,7 +1253,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:49:22</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1503,7 +1503,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1553,7 +1553,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1578,7 +1578,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1603,7 +1603,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1613,11 +1613,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,21 +1628,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:41</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,12 +1653,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1667,7 +1667,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,21 +1678,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1703,12 +1703,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:46</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1733,16 +1733,16 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,23 +1753,223 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>08:52</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>116</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>07:15:48</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>98</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>74</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
         <is>
           <t>08:57</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D57" t="n">
+      <c r="D60" t="n">
         <v>102</v>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>78</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>09:14</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>94</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>09:18</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>98</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>09:18</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>98</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>09:31</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>111</v>
+      </c>
+      <c r="E65" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1786,7 +1986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1804,14 +2004,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:15:48</t>
+          <t>Última actualización: 07:40:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 11</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
     </row>
@@ -1995,7 +2195,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2009,7 +2209,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2045,7 +2245,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2059,7 +2259,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2095,23 +2295,73 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>74</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>07:15:48</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>08:57</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="D17" t="n">
         <v>102</v>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>78</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2146,7 +2396,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:15:48</t>
+          <t>Última actualización: 07:40:11</t>
         </is>
       </c>
     </row>
@@ -2212,7 +2462,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2226,7 +2476,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -2262,7 +2512,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2276,7 +2526,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -2312,7 +2562,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2326,7 +2576,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 957
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:40:11</t>
+          <t>Última actualización: 07:52:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 60</t>
+          <t>Total filas: 67</t>
         </is>
       </c>
     </row>
@@ -1278,7 +1278,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1503,7 +1503,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1553,7 +1553,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1563,11 +1563,11 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1578,7 +1578,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1588,11 +1588,11 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1603,7 +1603,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1613,11 +1613,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1678,7 +1678,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1728,12 +1728,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:47</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,12 +1753,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1767,7 +1767,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1778,21 +1778,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,12 +1803,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1817,7 +1817,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,21 +1828,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,12 +1853,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1867,7 +1867,7 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1878,21 +1878,21 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>09:14</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,21 +1903,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,21 +1928,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:12</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1958,18 +1958,193 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
+          <t>09:14</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>94</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>07:52:32</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>85</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>09:18</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>98</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>07:52:32</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>09:18</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>86</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
           <t>09:31</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D65" t="n">
+      <c r="D69" t="n">
         <v>111</v>
       </c>
-      <c r="E65" t="inlineStr">
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>07:52:32</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>09:39</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>107</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>07:52:32</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>109</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>07:52:32</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>111</v>
+      </c>
+      <c r="E72" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2004,7 +2179,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:40:11</t>
+          <t>Última actualización: 07:52:32</t>
         </is>
       </c>
     </row>
@@ -2245,7 +2420,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2259,7 +2434,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2270,7 +2445,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2284,7 +2459,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2345,7 +2520,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2359,7 +2534,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2378,7 +2553,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2396,14 +2571,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:40:11</t>
+          <t>Última actualización: 07:52:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -2512,7 +2687,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2526,7 +2701,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -2562,7 +2737,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2576,11 +2751,36 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>07:52:32</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>89</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 958
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:52:32</t>
+          <t>Última actualización: 08:10:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 67</t>
+          <t>Total filas: 73</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1503,7 +1503,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1553,7 +1553,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1563,11 +1563,11 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1578,7 +1578,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1588,11 +1588,11 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1678,7 +1678,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1753,7 +1753,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1767,7 +1767,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1817,7 +1817,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1878,7 +1878,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,21 +1903,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,21 +1928,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>09:12</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,12 +1953,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>09:14</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1983,16 +1983,16 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:12</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2008,16 +2008,16 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:14</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2028,21 +2028,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2053,21 +2053,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>09:31</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2078,21 +2078,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2103,21 +2103,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,23 +2128,173 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
+          <t>09:36</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>86</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>08:10:22</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>09:39</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>89</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>08:10:22</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>91</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>08:10:22</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
           <t>09:43</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="C75" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D72" t="n">
-        <v>111</v>
-      </c>
-      <c r="E72" t="inlineStr">
+      <c r="D75" t="n">
+        <v>93</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>08:10:22</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>103</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>08:10:22</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>109</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>08:10:22</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>10:05</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>115</v>
+      </c>
+      <c r="E78" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2161,7 +2311,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2179,14 +2329,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:52:32</t>
+          <t>Última actualización: 08:10:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 14</t>
         </is>
       </c>
     </row>
@@ -2420,7 +2570,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2434,7 +2584,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2445,7 +2595,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2459,7 +2609,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2520,7 +2670,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2534,9 +2684,34 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>08:10:22</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>109</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2571,7 +2746,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:52:32</t>
+          <t>Última actualización: 08:10:22</t>
         </is>
       </c>
     </row>
@@ -2687,7 +2862,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2701,7 +2876,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -2737,7 +2912,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2751,7 +2926,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -2762,7 +2937,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2776,7 +2951,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 959
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:10:22</t>
+          <t>Última actualización: 08:30:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 73</t>
+          <t>Total filas: 81</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1603,21 +1603,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>08:41</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,21 +1628,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>08:41</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,21 +1653,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:41</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,21 +1678,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>08:41</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1703,21 +1703,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>08:46</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,21 +1728,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>08:47</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,12 +1753,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:46</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1767,7 +1767,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1778,12 +1778,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:47</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1808,16 +1808,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,21 +1828,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,21 +1853,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1878,21 +1878,21 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,21 +1903,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>09:05</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,21 +1928,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,21 +1953,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,21 +1978,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>09:12</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,21 +2003,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>09:14</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2033,16 +2033,16 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2053,21 +2053,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:12</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2083,16 +2083,16 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:14</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2103,21 +2103,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>09:31</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2133,16 +2133,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>09:36</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,21 +2153,21 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,21 +2178,21 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2203,21 +2203,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2233,16 +2233,16 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:36</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,21 +2253,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2283,18 +2283,218 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>91</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>72</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>73</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>83</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>89</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>08:10:22</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
           <t>10:05</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="C83" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D78" t="n">
+      <c r="D83" t="n">
         <v>115</v>
       </c>
-      <c r="E78" t="inlineStr">
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>10:06</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>96</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>103</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>10:24</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>114</v>
+      </c>
+      <c r="E86" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2329,7 +2529,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:10:22</t>
+          <t>Última actualización: 08:30:14</t>
         </is>
       </c>
     </row>
@@ -2570,7 +2770,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2584,7 +2784,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2620,7 +2820,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2634,7 +2834,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2670,7 +2870,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2684,7 +2884,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2695,7 +2895,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2709,7 +2909,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2728,7 +2928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2746,14 +2946,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:10:22</t>
+          <t>Última actualización: 08:30:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -2862,7 +3062,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2876,7 +3076,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -2912,7 +3112,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2926,7 +3126,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -2937,7 +3137,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2951,11 +3151,36 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>103</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 960
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:30:14</t>
+          <t>Última actualización: 08:40:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 81</t>
+          <t>Total filas: 93</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1653,12 +1653,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>08:41</t>
+          <t>08:40</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1667,7 +1667,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,12 +1678,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>08:41</t>
+          <t>08:40</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1703,21 +1703,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:41</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,21 +1728,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>08:41</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,21 +1753,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>08:46</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1778,21 +1778,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>08:47</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,12 +1803,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:46</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1817,7 +1817,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,12 +1828,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:47</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,21 +1853,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1878,12 +1878,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,12 +1903,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,21 +1928,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1958,16 +1958,16 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,21 +1978,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>09:05</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2008,16 +2008,16 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2028,21 +2028,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2053,21 +2053,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>09:12</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2078,21 +2078,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>09:14</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2103,12 +2103,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2117,7 +2117,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,21 +2128,21 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:12</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,21 +2153,21 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:14</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,21 +2178,21 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2203,21 +2203,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>09:31</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,21 +2228,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>09:36</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2258,16 +2258,16 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,21 +2278,21 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2308,16 +2308,16 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,21 +2328,21 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2353,21 +2353,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:10:22</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:36</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2378,21 +2378,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>09:38</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2403,21 +2403,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>10:05</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2428,21 +2428,21 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>10:06</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,21 +2453,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2483,18 +2483,318 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>72</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>73</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>09:52</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>72</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>83</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>78</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>89</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>10:05</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>85</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>10:06</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>96</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>92</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>103</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>101</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
           <t>10:24</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C97" t="inlineStr">
         <is>
           <t>23_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D86" t="n">
+      <c r="D97" t="n">
         <v>114</v>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>10:28</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>108</v>
+      </c>
+      <c r="E98" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2511,7 +2811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2529,14 +2829,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:30:14</t>
+          <t>Última actualización: 08:40:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 14</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -2745,7 +3045,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2759,7 +3059,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -2795,7 +3095,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2809,7 +3109,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2845,7 +3145,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2859,7 +3159,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2895,23 +3195,48 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>78</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>08:30:14</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>09:59</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D20" t="n">
         <v>89</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2928,7 +3253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2946,14 +3271,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:30:14</t>
+          <t>Última actualización: 08:40:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -3087,7 +3412,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3101,7 +3426,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -3137,12 +3462,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -3151,7 +3476,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -3167,20 +3492,120 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>51</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>92</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>10:13</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D15" t="n">
         <v>103</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>109</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>110</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 961
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:40:59</t>
+          <t>Última actualización: 08:52:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 93</t>
+          <t>Total filas: 96</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1878,7 +1878,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,7 +1903,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2017,7 +2017,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2067,7 +2067,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2078,7 +2078,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2092,7 +2092,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2178,7 +2178,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2192,7 +2192,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2403,7 +2403,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2417,7 +2417,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2503,7 +2503,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2567,7 +2567,7 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2603,7 +2603,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2617,7 +2617,7 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2628,7 +2628,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2642,7 +2642,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2703,7 +2703,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2717,7 +2717,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2728,7 +2728,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2795,6 +2795,81 @@
         <v>108</v>
       </c>
       <c r="E98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>97</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>112</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>10:46</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>15_P INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>114</v>
+      </c>
+      <c r="E101" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2829,7 +2904,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:40:59</t>
+          <t>Última actualización: 08:52:33</t>
         </is>
       </c>
     </row>
@@ -3095,7 +3170,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -3109,7 +3184,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -3170,7 +3245,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -3184,7 +3259,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -3220,7 +3295,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3234,7 +3309,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3253,7 +3328,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3271,14 +3346,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:40:59</t>
+          <t>Última actualización: 08:52:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -3462,37 +3537,37 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>09:20</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -3501,7 +3576,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -3512,37 +3587,37 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3551,7 +3626,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -3562,25 +3637,25 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10:29</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
@@ -3592,18 +3667,93 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>109</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>10:30</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>98</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D19" t="n">
         <v>110</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>10:31</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>99</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 962
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:52:33</t>
+          <t>Última actualización: 09:23:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 96</t>
+          <t>Total filas: 106</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2353,7 +2353,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>08:10:22</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2367,7 +2367,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2403,7 +2403,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2417,7 +2417,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2503,7 +2503,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2567,7 +2567,7 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2578,7 +2578,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2628,7 +2628,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2642,7 +2642,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2703,7 +2703,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2717,7 +2717,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2728,12 +2728,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2753,12 +2753,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>10:24</t>
+          <t>10:21</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2767,7 +2767,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2778,21 +2778,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>10:28</t>
+          <t>10:24</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2803,21 +2803,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>10:29</t>
+          <t>10:25</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,21 +2828,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>10:44</t>
+          <t>10:28</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,23 +2853,273 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>66</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>66</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>10:43</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>80</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
           <t>08:52:33</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr">
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>112</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
         <is>
           <t>10:46</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
+      <c r="C105" t="inlineStr">
         <is>
           <t>15_P INDUSTRIAL</t>
         </is>
       </c>
-      <c r="D101" t="n">
-        <v>114</v>
-      </c>
-      <c r="E101" t="inlineStr">
+      <c r="D105" t="n">
+        <v>83</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>10:53</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>90</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>98</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>98</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>107</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>112</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>116</v>
+      </c>
+      <c r="E111" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2904,7 +3154,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:52:33</t>
+          <t>Última actualización: 09:23:52</t>
         </is>
       </c>
     </row>
@@ -3270,7 +3520,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3284,7 +3534,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -3328,7 +3578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3346,14 +3596,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:52:33</t>
+          <t>Última actualización: 09:23:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
     </row>
@@ -3612,37 +3862,37 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -3651,7 +3901,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -3662,37 +3912,37 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10:29</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>10:29</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -3701,7 +3951,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -3712,7 +3962,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3726,7 +3976,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -3742,18 +3992,43 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>98</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>10:31</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>99</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 963
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:23:52</t>
+          <t>Última actualización: 10:07:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 106</t>
+          <t>Total filas: 119</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2703,7 +2703,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2717,7 +2717,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2778,12 +2778,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>10:24</t>
+          <t>10:22</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2792,7 +2792,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>114</v>
+        <v>15</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2803,21 +2803,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>10:25</t>
+          <t>10:24</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,21 +2828,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>10:28</t>
+          <t>10:25</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,21 +2853,21 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>10:29</t>
+          <t>10:28</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,21 +2903,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>10:43</t>
+          <t>10:29</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,12 +2928,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>10:44</t>
+          <t>10:43</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2942,7 +2942,7 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2953,21 +2953,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>10:46</t>
+          <t>10:44</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>15_P INDUSTRIAL</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2978,21 +2978,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>10:53</t>
+          <t>10:46</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_P INDUSTRIAL</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3008,16 +3008,16 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:53</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3028,21 +3028,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:56</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3053,21 +3053,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>11:10</t>
+          <t>10:59</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3083,16 +3083,16 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>11:01</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,23 +3103,348 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>54</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>11:03</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>56</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>63</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>67</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>68</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
           <t>09:23:52</t>
         </is>
       </c>
-      <c r="B111" t="inlineStr">
+      <c r="B116" t="inlineStr">
         <is>
           <t>11:19</t>
         </is>
       </c>
-      <c r="C111" t="inlineStr">
+      <c r="C116" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D111" t="n">
+      <c r="D116" t="n">
         <v>116</v>
       </c>
-      <c r="E111" t="inlineStr">
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>74</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>11:29</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>82</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>83</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>94</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>98</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>105</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>111</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>12:05</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>118</v>
+      </c>
+      <c r="E124" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3136,7 +3461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3154,14 +3479,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:23:52</t>
+          <t>Última actualización: 10:07:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -3562,6 +3887,56 @@
         <v>67</v>
       </c>
       <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>83</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>94</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3578,7 +3953,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3596,14 +3971,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:23:52</t>
+          <t>Última actualización: 10:07:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -3887,7 +4262,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3901,7 +4276,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -3937,7 +4312,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -3951,7 +4326,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -3962,7 +4337,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3972,11 +4347,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -3987,7 +4362,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3997,11 +4372,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -4031,6 +4406,31 @@
       <c r="E21" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>10:07:51</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:25</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>78</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 964
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:07:51</t>
+          <t>Última actualización: 10:41:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 119</t>
+          <t>Total filas: 130</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2953,7 +2953,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2967,7 +2967,7 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>112</v>
+        <v>3</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2978,7 +2978,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2992,7 +2992,7 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3028,21 +3028,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>10:56</t>
+          <t>10:55</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3053,21 +3053,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>10:59</t>
+          <t>10:56</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3078,12 +3078,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:59</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3092,7 +3092,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3128,21 +3128,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>11:03</t>
+          <t>11:01</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3158,16 +3158,16 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>11:10</t>
+          <t>11:03</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3178,21 +3178,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>11:14</t>
+          <t>11:07</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3203,21 +3203,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>11:10</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3228,21 +3228,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>11:14</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3253,21 +3253,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>11:21</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3278,12 +3278,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>11:29</t>
+          <t>11:19</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3292,7 +3292,7 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3308,16 +3308,16 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:21</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3328,21 +3328,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3353,21 +3353,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>11:29</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3378,21 +3378,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>105</v>
+        <v>49</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,21 +3403,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3428,23 +3428,298 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>64</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>11:49</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>68</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
           <t>10:07:51</t>
         </is>
       </c>
-      <c r="B124" t="inlineStr">
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>105</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>11:53</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>72</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>77</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
         <is>
           <t>12:05</t>
         </is>
       </c>
-      <c r="C124" t="inlineStr">
+      <c r="C129" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D124" t="n">
-        <v>118</v>
-      </c>
-      <c r="E124" t="inlineStr">
+      <c r="D129" t="n">
+        <v>84</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>89</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>89</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>100</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>12:32</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>111</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>113</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>115</v>
+      </c>
+      <c r="E135" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3461,7 +3736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3479,14 +3754,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:07:51</t>
+          <t>Última actualización: 10:41:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
     </row>
@@ -3895,7 +4170,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3909,7 +4184,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -3920,7 +4195,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3934,9 +4209,34 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>100</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3971,7 +4271,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:07:51</t>
+          <t>Última actualización: 10:41:48</t>
         </is>
       </c>
     </row>
@@ -4412,7 +4712,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4426,7 +4726,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 965
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:41:48</t>
+          <t>Última actualización: 10:56:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 130</t>
+          <t>Total filas: 140</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3078,21 +3078,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>10:59</t>
+          <t>10:57</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,12 +3103,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:59</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3117,7 +3117,7 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>98</v>
+        <v>3</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,21 +3153,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>11:03</t>
+          <t>11:01</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3178,12 +3178,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>11:07</t>
+          <t>11:03</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3192,7 +3192,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3203,21 +3203,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>11:10</t>
+          <t>11:07</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3228,21 +3228,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>11:14</t>
+          <t>11:10</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3258,16 +3258,16 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>11:14</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3278,21 +3278,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>116</v>
+        <v>19</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,21 +3303,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>11:21</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3328,21 +3328,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>11:25</t>
+          <t>11:19</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3353,21 +3353,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>11:29</t>
+          <t>11:21</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3378,21 +3378,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,21 +3403,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:29</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3433,16 +3433,16 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3453,21 +3453,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>11:49</t>
+          <t>11:31</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3478,21 +3478,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,21 +3503,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:42</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3528,21 +3528,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,21 +3553,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3583,16 +3583,16 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>11:49</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3603,21 +3603,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,21 +3628,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,21 +3653,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3683,16 +3683,16 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,23 +3703,273 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>70</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>74</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>74</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
           <t>10:41:48</t>
         </is>
       </c>
-      <c r="B135" t="inlineStr">
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>100</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>86</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>12:32</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>111</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>12:33</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>97</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>98</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>98</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
         <is>
           <t>12:36</t>
         </is>
       </c>
-      <c r="C135" t="inlineStr">
+      <c r="C144" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D135" t="n">
+      <c r="D144" t="n">
         <v>115</v>
       </c>
-      <c r="E135" t="inlineStr">
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>112</v>
+      </c>
+      <c r="E145" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3731,6 +3981,598 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 25/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 10:56:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 21</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>28</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:44</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>14</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>24</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>17</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>35</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>67</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>49</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>35</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>60</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>46</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>100</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10:56:01</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>86</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3747,14 +4589,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 25/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 25/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:41:48</t>
+          <t>Última actualización: 10:56:01</t>
         </is>
       </c>
     </row>
@@ -3795,175 +4637,175 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:16</t>
+          <t>07:42</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>08:36</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>07:44</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
@@ -3975,220 +4817,220 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>10:29</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>10:31</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -4200,535 +5042,43 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>11:26</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="E23" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 25/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 10:41:48</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 17</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>07:15:48</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>07:42</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>27</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>07:40:11</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>07:43</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>07:15:48</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>08:35</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>80</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>08:30:14</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>08:36</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>6</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>08:40:59</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>08:50</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>10</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>08:30:14</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>08:51</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>21</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>08:52</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>08:40:59</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>09:20</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>40</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>09:21</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>29</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>09:23:52</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>09:23</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>10:07:51</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>10:12</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>5</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>10:13</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>81</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>10:07:51</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>10:29</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>22</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>98</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>10:07:51</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>23</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>10:31</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>99</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>10:41:48</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>11:25</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>44</v>
-      </c>
-      <c r="E22" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 966
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:56:01</t>
+          <t>Última actualización: 11:13:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 140</t>
+          <t>Total filas: 145</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3292,7 +3292,7 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3317,7 +3317,7 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3392,7 +3392,7 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3417,7 +3417,7 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3453,7 +3453,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3467,7 +3467,7 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3517,7 +3517,7 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,12 +3628,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3642,7 +3642,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,21 +3653,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,21 +3678,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,12 +3703,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3717,7 +3717,7 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3728,21 +3728,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3753,7 +3753,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3767,7 +3767,7 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3778,21 +3778,21 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3803,21 +3803,21 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3833,16 +3833,16 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,21 +3853,21 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3878,21 +3878,21 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,21 +3903,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3928,21 +3928,21 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3953,23 +3953,148 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
+          <t>11:13:01</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>12:33</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>80</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>11:13:01</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>81</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
           <t>10:56:01</t>
         </is>
       </c>
-      <c r="B145" t="inlineStr">
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>98</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>115</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>11:13:01</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
         <is>
           <t>12:48</t>
         </is>
       </c>
-      <c r="C145" t="inlineStr">
+      <c r="C149" t="inlineStr">
         <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D145" t="n">
-        <v>112</v>
-      </c>
-      <c r="E145" t="inlineStr">
+      <c r="D149" t="n">
+        <v>95</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>11:13:01</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>110</v>
+      </c>
+      <c r="E150" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4004,7 +4129,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:56:01</t>
+          <t>Última actualización: 11:13:01</t>
         </is>
       </c>
     </row>
@@ -4445,7 +4570,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4459,7 +4584,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -4495,7 +4620,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -4509,7 +4634,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -4545,7 +4670,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4559,7 +4684,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -4596,7 +4721,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:56:01</t>
+          <t>Última actualización: 11:13:01</t>
         </is>
       </c>
     </row>
@@ -5062,7 +5187,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -5076,7 +5201,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 967
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:13:01</t>
+          <t>Última actualización: 11:35:40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 145</t>
+          <t>Total filas: 155</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3478,7 +3478,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,21 +3678,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,21 +3703,21 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3728,12 +3728,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3742,7 +3742,7 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3758,16 +3758,16 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3803,21 +3803,21 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3828,21 +3828,21 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,12 +3853,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -3867,7 +3867,7 @@
         </is>
       </c>
       <c r="D141" t="n">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3883,16 +3883,16 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,21 +3903,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3933,16 +3933,16 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3953,21 +3953,21 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3983,16 +3983,16 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4003,21 +4003,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,12 +4028,12 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4042,7 +4042,7 @@
         </is>
       </c>
       <c r="D148" t="n">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,21 +4053,21 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4078,23 +4078,273 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>61</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>12:47</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>72</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>73</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>73</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>87</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>88</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
           <t>11:13:01</t>
         </is>
       </c>
-      <c r="B150" t="inlineStr">
+      <c r="B156" t="inlineStr">
         <is>
           <t>13:03</t>
         </is>
       </c>
-      <c r="C150" t="inlineStr">
+      <c r="C156" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D150" t="n">
+      <c r="D156" t="n">
         <v>110</v>
       </c>
-      <c r="E150" t="inlineStr">
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>98</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>102</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>110</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>118</v>
+      </c>
+      <c r="E160" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4111,7 +4361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4129,14 +4379,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:13:01</t>
+          <t>Última actualización: 11:35:40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -4595,7 +4845,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4609,7 +4859,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -4645,7 +4895,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4659,7 +4909,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -4687,6 +4937,56 @@
         <v>69</v>
       </c>
       <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>88</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>118</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4703,7 +5003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4721,14 +5021,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:13:01</t>
+          <t>Última actualización: 11:35:40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -5087,7 +5387,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -5097,11 +5397,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -5112,7 +5412,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -5122,11 +5422,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -5206,6 +5506,56 @@
       <c r="E23" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>13:11</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>96</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>105</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 968
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:35:40</t>
+          <t>Última actualización: 11:48:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 155</t>
+          <t>Total filas: 159</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3578,21 +3578,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>11:49</t>
+          <t>11:48</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3603,21 +3603,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>11:49</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3642,7 +3642,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,21 +3653,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3703,21 +3703,21 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3728,21 +3728,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3753,12 +3753,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3767,7 +3767,7 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3778,21 +3778,21 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3803,7 +3803,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -3817,7 +3817,7 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3828,21 +3828,21 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,21 +3853,21 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3878,12 +3878,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,21 +3903,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3958,16 +3958,16 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3978,21 +3978,21 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4003,21 +4003,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,21 +4028,21 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,21 +4053,21 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4078,21 +4078,21 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4103,21 +4103,21 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4133,16 +4133,16 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,21 +4153,21 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,21 +4178,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4203,21 +4203,21 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4228,21 +4228,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4253,21 +4253,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4278,21 +4278,21 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4308,16 +4308,16 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4328,23 +4328,123 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
+          <t>11:48:20</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>76</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
           <t>11:35:40</t>
         </is>
       </c>
-      <c r="B160" t="inlineStr">
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>98</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>11:48:20</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>89</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>11:48:20</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>97</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>11:48:20</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
         <is>
           <t>13:33</t>
         </is>
       </c>
-      <c r="C160" t="inlineStr">
+      <c r="C164" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D160" t="n">
-        <v>118</v>
-      </c>
-      <c r="E160" t="inlineStr">
+      <c r="D164" t="n">
+        <v>105</v>
+      </c>
+      <c r="E164" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4361,7 +4461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4379,14 +4479,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:35:40</t>
+          <t>Última actualización: 11:48:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -4920,7 +5020,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4934,7 +5034,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -4970,23 +5070,48 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>76</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>11:48:20</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>13:33</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D28" t="n">
-        <v>118</v>
-      </c>
-      <c r="E28" t="inlineStr">
+      <c r="D29" t="n">
+        <v>105</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5003,7 +5128,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5021,14 +5146,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:35:40</t>
+          <t>Última actualización: 11:48:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -5537,23 +5662,73 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>11:48:20</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>13:12</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>84</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>11:35:40</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>13:20</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="D26" t="n">
         <v>105</v>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11:48:20</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>93</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 969
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:48:20</t>
+          <t>Última actualización: 11:55:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 159</t>
+          <t>Total filas: 165</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3728,21 +3728,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:55</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3753,21 +3753,21 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3778,12 +3778,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3792,7 +3792,7 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3803,21 +3803,21 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3842,7 +3842,7 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,21 +3853,21 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3878,21 +3878,21 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,12 +3903,12 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -3917,7 +3917,7 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3928,21 +3928,21 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3953,7 +3953,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -3963,11 +3963,11 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3978,12 +3978,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -3992,7 +3992,7 @@
         </is>
       </c>
       <c r="D146" t="n">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4028,21 +4028,21 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4078,21 +4078,21 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4128,21 +4128,21 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,12 +4153,12 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -4167,7 +4167,7 @@
         </is>
       </c>
       <c r="D153" t="n">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,21 +4178,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4203,21 +4203,21 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4233,16 +4233,16 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4253,21 +4253,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4278,21 +4278,21 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>110</v>
+        <v>53</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4303,21 +4303,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4333,16 +4333,16 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,21 +4353,21 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,21 +4378,21 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4403,21 +4403,21 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4428,23 +4428,173 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>78</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>11:55:01</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>82</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>11:55:01</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>13:24</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>89</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>11:55:01</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>90</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>11:55:01</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
           <t>13:33</t>
         </is>
       </c>
-      <c r="C164" t="inlineStr">
+      <c r="C168" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D164" t="n">
-        <v>105</v>
-      </c>
-      <c r="E164" t="inlineStr">
+      <c r="D168" t="n">
+        <v>98</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>11:55:01</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>13:47</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>112</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>11:55:01</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>13:49</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>114</v>
+      </c>
+      <c r="E170" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4479,7 +4629,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:48:20</t>
+          <t>Última actualización: 11:55:01</t>
         </is>
       </c>
     </row>
@@ -5020,7 +5170,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -5034,7 +5184,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -5070,7 +5220,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -5084,7 +5234,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -5095,7 +5245,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -5109,7 +5259,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -5146,7 +5296,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:48:20</t>
+          <t>Última actualización: 11:55:01</t>
         </is>
       </c>
     </row>
@@ -5662,7 +5812,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -5676,7 +5826,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -5712,7 +5862,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -5726,7 +5876,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 970
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E170"/>
+  <dimension ref="A1:E173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:55:01</t>
+          <t>Última actualización: 12:12:04</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 165</t>
+          <t>Total filas: 168</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -3878,21 +3878,21 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:12</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,21 +3903,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3928,21 +3928,21 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3953,21 +3953,21 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3978,21 +3978,21 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4003,21 +4003,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,12 +4028,12 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4042,7 +4042,7 @@
         </is>
       </c>
       <c r="D148" t="n">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,12 +4053,12 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4067,7 +4067,7 @@
         </is>
       </c>
       <c r="D149" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4078,12 +4078,12 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4092,7 +4092,7 @@
         </is>
       </c>
       <c r="D150" t="n">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4103,21 +4103,21 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,21 +4128,21 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,21 +4153,21 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,21 +4178,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4203,12 +4203,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -4217,7 +4217,7 @@
         </is>
       </c>
       <c r="D155" t="n">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4228,21 +4228,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4253,21 +4253,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4278,21 +4278,21 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4303,7 +4303,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -4313,11 +4313,11 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4328,21 +4328,21 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4358,16 +4358,16 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,21 +4378,21 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4403,21 +4403,21 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4428,21 +4428,21 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,21 +4453,21 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4483,16 +4483,16 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4503,21 +4503,21 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:17</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,21 +4528,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4553,21 +4553,21 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,23 +4578,98 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>81</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>81</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>13:47</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>95</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
           <t>11:55:01</t>
         </is>
       </c>
-      <c r="B170" t="inlineStr">
+      <c r="B173" t="inlineStr">
         <is>
           <t>13:49</t>
         </is>
       </c>
-      <c r="C170" t="inlineStr">
+      <c r="C173" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D170" t="n">
+      <c r="D173" t="n">
         <v>114</v>
       </c>
-      <c r="E170" t="inlineStr">
+      <c r="E173" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4629,7 +4704,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:55:01</t>
+          <t>Última actualización: 12:12:04</t>
         </is>
       </c>
     </row>
@@ -5170,7 +5245,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -5184,7 +5259,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -5220,7 +5295,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -5234,7 +5309,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -5245,7 +5320,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -5259,7 +5334,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -5278,7 +5353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5296,14 +5371,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:55:01</t>
+          <t>Última actualización: 12:12:04</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -5662,7 +5737,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -5672,11 +5747,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -5687,7 +5762,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -5697,11 +5772,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -5812,7 +5887,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -5826,7 +5901,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -5862,7 +5937,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -5876,11 +5951,36 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>105</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 971
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E173"/>
+  <dimension ref="A1:E183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:12:04</t>
+          <t>Última actualización: 12:33:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 168</t>
+          <t>Total filas: 178</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4167,7 +4167,7 @@
         </is>
       </c>
       <c r="D153" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4203,7 +4203,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -4213,11 +4213,11 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4228,12 +4228,12 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -4242,7 +4242,7 @@
         </is>
       </c>
       <c r="D156" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4278,21 +4278,21 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4303,21 +4303,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,21 +4378,21 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4403,12 +4403,12 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -4417,7 +4417,7 @@
         </is>
       </c>
       <c r="D163" t="n">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,12 +4453,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -4467,7 +4467,7 @@
         </is>
       </c>
       <c r="D165" t="n">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4478,21 +4478,21 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4503,21 +4503,21 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,21 +4528,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:17</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4553,21 +4553,21 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4583,16 +4583,16 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4603,21 +4603,21 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,21 +4628,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,23 +4653,273 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>59</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>81</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>81</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>73</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>13:47</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>95</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
           <t>11:55:01</t>
         </is>
       </c>
-      <c r="B173" t="inlineStr">
+      <c r="B178" t="inlineStr">
         <is>
           <t>13:49</t>
         </is>
       </c>
-      <c r="C173" t="inlineStr">
+      <c r="C178" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D173" t="n">
+      <c r="D178" t="n">
         <v>114</v>
       </c>
-      <c r="E173" t="inlineStr">
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>81</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>14:01</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>88</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>103</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>104</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>14:31</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>118</v>
+      </c>
+      <c r="E183" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4681,6 +4931,698 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 25/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 12:33:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>28</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:44</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>14</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>24</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>17</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>35</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>67</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>49</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>11:13:01</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>18</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>6</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>11:13:01</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>29</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>46</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>30</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>52</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>59</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>81</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4697,14 +5639,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 25/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 25/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:12:04</t>
+          <t>Última actualización: 12:33:54</t>
         </is>
       </c>
     </row>
@@ -4745,175 +5687,175 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:58:04</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:16</t>
+          <t>07:42</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:40:11</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>08:36</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>07:40:11</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>07:44</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
@@ -4925,170 +5867,170 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>10:29</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -5100,220 +6042,220 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>10:41:48</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>10:31</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>10:41:48</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11:31</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:26</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>13:11</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>13:12</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:56</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
@@ -5325,660 +6267,18 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="E29" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 25/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 12:12:04</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 23</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>07:15:48</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>07:42</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>27</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>07:40:11</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>07:43</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>07:15:48</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>08:35</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>80</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>08:30:14</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>08:36</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>6</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>08:40:59</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>08:50</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>10</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>08:30:14</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>08:51</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>21</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>08:52</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>08:40:59</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>09:20</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>40</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>09:21</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>29</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>09:23:52</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>09:23</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>10:07:51</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>10:12</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>5</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>10:13</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>81</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>10:07:51</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>10:29</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>22</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>98</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>10:07:51</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>23</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>10:31</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>99</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>10:41:48</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>11:25</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>44</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>11:13:01</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>11:26</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>13</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>11:35:40</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>13:11</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>96</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>12:12:04</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>13:12</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>60</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>11:35:40</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>13:20</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>105</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>12:12:04</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>13:21</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>69</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>12:12:04</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>13:57</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>105</v>
-      </c>
-      <c r="E28" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 972
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E183"/>
+  <dimension ref="A1:E194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:33:54</t>
+          <t>Última actualización: 12:47:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 178</t>
+          <t>Total filas: 189</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4303,7 +4303,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -4317,7 +4317,7 @@
         </is>
       </c>
       <c r="D159" t="n">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4367,7 +4367,7 @@
         </is>
       </c>
       <c r="D161" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4442,7 +4442,7 @@
         </is>
       </c>
       <c r="D164" t="n">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4478,7 +4478,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -4492,7 +4492,7 @@
         </is>
       </c>
       <c r="D166" t="n">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4542,7 +4542,7 @@
         </is>
       </c>
       <c r="D168" t="n">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4553,21 +4553,21 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,12 +4578,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -4592,7 +4592,7 @@
         </is>
       </c>
       <c r="D170" t="n">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4603,21 +4603,21 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:22</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,21 +4628,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:12:04</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,21 +4653,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,12 +4678,12 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -4692,7 +4692,7 @@
         </is>
       </c>
       <c r="D174" t="n">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,12 +4703,12 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -4717,7 +4717,7 @@
         </is>
       </c>
       <c r="D175" t="n">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4728,21 +4728,21 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,21 +4753,21 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,21 +4778,21 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>13:49</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,21 +4803,21 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:47</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4828,21 +4828,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:49</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4853,21 +4853,21 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,21 +4878,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>13:58</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4908,18 +4908,293 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
+          <t>14:01</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>88</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>14:02</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>75</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>14:07</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>80</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>103</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>104</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>90</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>14:18</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>91</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>100</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
           <t>14:31</t>
         </is>
       </c>
-      <c r="C183" t="inlineStr">
+      <c r="C191" t="inlineStr">
         <is>
           <t>14X44_ABASTO</t>
         </is>
       </c>
-      <c r="D183" t="n">
+      <c r="D191" t="n">
         <v>118</v>
       </c>
-      <c r="E183" t="inlineStr">
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>14:32</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>105</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>107</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>112</v>
+      </c>
+      <c r="E194" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4936,7 +5211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4954,14 +5229,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:33:54</t>
+          <t>Última actualización: 12:47:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -5545,7 +5820,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -5559,7 +5834,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -5595,7 +5870,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5609,9 +5884,34 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>107</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5646,7 +5946,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:33:54</t>
+          <t>Última actualización: 12:47:00</t>
         </is>
       </c>
     </row>
@@ -6012,7 +6312,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -6022,11 +6322,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -6037,7 +6337,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -6047,11 +6347,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -6162,7 +6462,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -6176,7 +6476,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -6212,7 +6512,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -6226,7 +6526,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -6262,7 +6562,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>12:12:04</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -6276,7 +6576,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 973
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E194"/>
+  <dimension ref="A1:E199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:47:00</t>
+          <t>Última actualización: 12:54:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 189</t>
+          <t>Total filas: 194</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4403,7 +4403,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -4417,7 +4417,7 @@
         </is>
       </c>
       <c r="D163" t="n">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4503,7 +4503,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4517,7 +4517,7 @@
         </is>
       </c>
       <c r="D167" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4542,7 +4542,7 @@
         </is>
       </c>
       <c r="D168" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4567,7 +4567,7 @@
         </is>
       </c>
       <c r="D169" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4592,7 +4592,7 @@
         </is>
       </c>
       <c r="D170" t="n">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4667,7 +4667,7 @@
         </is>
       </c>
       <c r="D173" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4688,7 +4688,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4738,7 +4738,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D176" t="n">
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4817,7 +4817,7 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4867,7 +4867,7 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,12 +4878,12 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>13:58</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -4892,7 +4892,7 @@
         </is>
       </c>
       <c r="D182" t="n">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4903,21 +4903,21 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:58</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4928,12 +4928,12 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>14:02</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="D184" t="n">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,21 +4953,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>14:07</t>
+          <t>14:02</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4978,21 +4978,21 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:06</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,21 +5003,21 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:07</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,12 +5028,12 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -5042,7 +5042,7 @@
         </is>
       </c>
       <c r="D188" t="n">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5053,12 +5053,12 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>14:18</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -5067,7 +5067,7 @@
         </is>
       </c>
       <c r="D189" t="n">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5083,16 +5083,16 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5103,21 +5103,21 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>14:31</t>
+          <t>14:18</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5133,16 +5133,16 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>14:32</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5153,21 +5153,21 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:31</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,23 +5178,148 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
+          <t>12:54:41</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>14:32</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>98</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>12:54:41</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>99</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
           <t>12:47:00</t>
         </is>
       </c>
-      <c r="B194" t="inlineStr">
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>107</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>12:54:41</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
         <is>
           <t>14:39</t>
         </is>
       </c>
-      <c r="C194" t="inlineStr">
+      <c r="C197" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D194" t="n">
-        <v>112</v>
-      </c>
-      <c r="E194" t="inlineStr">
+      <c r="D197" t="n">
+        <v>105</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>12:54:41</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>113</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>12:54:41</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>119</v>
+      </c>
+      <c r="E199" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5211,7 +5336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5229,14 +5354,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:47:00</t>
+          <t>Última actualización: 12:54:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -5795,7 +5920,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -5809,7 +5934,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -5870,7 +5995,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5884,7 +6009,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -5895,23 +6020,98 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>12:54:41</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>99</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>12:47:00</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>14:34</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="D32" t="n">
         <v>107</v>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>12:54:41</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>113</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>12:54:41</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>119</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5946,7 +6146,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:47:00</t>
+          <t>Última actualización: 12:54:41</t>
         </is>
       </c>
     </row>
@@ -6312,7 +6512,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -6322,11 +6522,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -6337,7 +6537,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -6347,11 +6547,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -6437,7 +6637,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -6451,7 +6651,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -6487,7 +6687,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -6501,7 +6701,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -6537,7 +6737,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -6551,7 +6751,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 974
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:54:41</t>
+          <t>Última actualización: 13:14:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 194</t>
+          <t>Total filas: 199</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4542,7 +4542,7 @@
         </is>
       </c>
       <c r="D168" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4567,7 +4567,7 @@
         </is>
       </c>
       <c r="D169" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4592,7 +4592,7 @@
         </is>
       </c>
       <c r="D170" t="n">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4667,7 +4667,7 @@
         </is>
       </c>
       <c r="D173" t="n">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4817,7 +4817,7 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4867,7 +4867,7 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4978,21 +4978,21 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>14:06</t>
+          <t>14:02</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,21 +5003,21 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>14:07</t>
+          <t>14:02</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5033,16 +5033,16 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:06</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5053,21 +5053,21 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:07</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5078,12 +5078,12 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -5092,7 +5092,7 @@
         </is>
       </c>
       <c r="D190" t="n">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5108,16 +5108,16 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>14:18</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5128,21 +5128,21 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5153,21 +5153,21 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>14:31</t>
+          <t>14:18</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,21 +5178,21 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>14:32</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,21 +5203,21 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:31</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5228,21 +5228,21 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:32</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5253,21 +5253,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5278,21 +5278,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5303,23 +5303,148 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>85</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>13:14:41</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>93</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>13:14:41</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
           <t>14:53</t>
         </is>
       </c>
-      <c r="C199" t="inlineStr">
+      <c r="C201" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D199" t="n">
+      <c r="D201" t="n">
+        <v>99</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>13:14:41</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>108</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>13:14:41</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>15:11</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>117</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>13:14:41</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
         <v>119</v>
       </c>
-      <c r="E199" t="inlineStr">
+      <c r="E204" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5354,7 +5479,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:54:41</t>
+          <t>Última actualización: 13:14:41</t>
         </is>
       </c>
     </row>
@@ -5995,7 +6120,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -6009,7 +6134,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -6020,7 +6145,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -6034,7 +6159,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -6070,7 +6195,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -6084,7 +6209,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -6095,7 +6220,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -6109,7 +6234,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -6128,7 +6253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6146,14 +6271,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:54:41</t>
+          <t>Última actualización: 13:14:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -6687,37 +6812,37 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:16</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -6726,7 +6851,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -6737,48 +6862,73 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>13:14:41</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>42</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>12:47:00</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>13:57</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D30" t="n">
         <v>70</v>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 975
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E204"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:14:41</t>
+          <t>Última actualización: 13:43:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 199</t>
+          <t>Total filas: 206</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4778,12 +4778,12 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:43</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -4792,7 +4792,7 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,12 +4803,12 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -4817,7 +4817,7 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4828,21 +4828,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>13:49</t>
+          <t>13:47</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4853,21 +4853,21 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:49</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,21 +4878,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>13:57</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4903,12 +4903,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>13:58</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -4917,7 +4917,7 @@
         </is>
       </c>
       <c r="D183" t="n">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4928,21 +4928,21 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:58</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,21 +4953,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>14:02</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4992,7 +4992,7 @@
         </is>
       </c>
       <c r="D186" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5013,7 +5013,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D187" t="n">
@@ -5028,21 +5028,21 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>14:06</t>
+          <t>14:02</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5053,12 +5053,12 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>14:07</t>
+          <t>14:06</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -5067,7 +5067,7 @@
         </is>
       </c>
       <c r="D189" t="n">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5078,21 +5078,21 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:07</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5103,21 +5103,21 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:14</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5133,16 +5133,16 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5153,12 +5153,12 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>14:18</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -5167,7 +5167,7 @@
         </is>
       </c>
       <c r="D193" t="n">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,21 +5178,21 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,21 +5203,21 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>14:31</t>
+          <t>14:18</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5228,21 +5228,21 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>14:32</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5253,21 +5253,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:31</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5278,21 +5278,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:32</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5308,16 +5308,16 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,21 +5328,21 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5353,21 +5353,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:39</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,21 +5378,21 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:47</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5403,21 +5403,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>15:11</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5433,18 +5433,193 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>99</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>13:43:25</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>71</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>13:43:25</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>79</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>13:14:41</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>15:11</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>117</v>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>13:43:25</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
           <t>15:13</t>
         </is>
       </c>
-      <c r="C204" t="inlineStr">
+      <c r="C208" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D204" t="n">
-        <v>119</v>
-      </c>
-      <c r="E204" t="inlineStr">
+      <c r="D208" t="n">
+        <v>90</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>13:43:25</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>15:17</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>94</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>13:43:25</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>111</v>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>13:43:25</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>15:41</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>118</v>
+      </c>
+      <c r="E211" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5461,7 +5636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5479,14 +5654,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:14:41</t>
+          <t>Última actualización: 13:43:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 31</t>
         </is>
       </c>
     </row>
@@ -6170,7 +6345,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -6184,7 +6359,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -6195,7 +6370,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -6209,7 +6384,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -6237,6 +6412,56 @@
         <v>99</v>
       </c>
       <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>13:43:25</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>71</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>13:43:25</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>111</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6253,7 +6478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6271,14 +6496,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:14:41</t>
+          <t>Última actualización: 13:43:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 27</t>
         </is>
       </c>
     </row>
@@ -6637,7 +6862,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -6647,11 +6872,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -6662,7 +6887,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -6672,11 +6897,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -6912,7 +7137,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -6926,11 +7151,61 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>13:43:25</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>44</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>13:43:25</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>15:22</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>99</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 976
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E211"/>
+  <dimension ref="A1:E215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:43:25</t>
+          <t>Última actualización: 13:57:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 206</t>
+          <t>Total filas: 210</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5053,7 +5053,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -5067,7 +5067,7 @@
         </is>
       </c>
       <c r="D189" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5103,7 +5103,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5117,7 +5117,7 @@
         </is>
       </c>
       <c r="D191" t="n">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5128,7 +5128,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -5142,7 +5142,7 @@
         </is>
       </c>
       <c r="D192" t="n">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5163,7 +5163,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D193" t="n">
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5228,7 +5228,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -5242,7 +5242,7 @@
         </is>
       </c>
       <c r="D196" t="n">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5278,7 +5278,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -5292,7 +5292,7 @@
         </is>
       </c>
       <c r="D198" t="n">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -5342,7 +5342,7 @@
         </is>
       </c>
       <c r="D200" t="n">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5353,7 +5353,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -5367,7 +5367,7 @@
         </is>
       </c>
       <c r="D201" t="n">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,7 +5378,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -5392,7 +5392,7 @@
         </is>
       </c>
       <c r="D202" t="n">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5403,7 +5403,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -5417,7 +5417,7 @@
         </is>
       </c>
       <c r="D203" t="n">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5428,21 +5428,21 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5453,12 +5453,12 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -5467,7 +5467,7 @@
         </is>
       </c>
       <c r="D205" t="n">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5478,21 +5478,21 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:54</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5503,21 +5503,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>15:11</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,21 +5528,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:11</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,21 +5553,21 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5578,21 +5578,21 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,23 +5603,123 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>97</v>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>13:57:31</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
           <t>15:41</t>
         </is>
       </c>
-      <c r="C211" t="inlineStr">
+      <c r="C212" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D211" t="n">
-        <v>118</v>
-      </c>
-      <c r="E211" t="inlineStr">
+      <c r="D212" t="n">
+        <v>104</v>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>13:57:31</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>116</v>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>13:57:31</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>116</v>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>13:57:31</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>119</v>
+      </c>
+      <c r="E215" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5654,7 +5754,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:43:25</t>
+          <t>Última actualización: 13:57:31</t>
         </is>
       </c>
     </row>
@@ -6345,7 +6445,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -6359,7 +6459,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -6370,7 +6470,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -6384,7 +6484,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -6420,7 +6520,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -6434,7 +6534,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -6445,7 +6545,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -6459,7 +6559,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -6478,7 +6578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6496,14 +6596,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:43:25</t>
+          <t>Última actualización: 13:57:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 27</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -7162,12 +7262,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>13:58</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -7176,7 +7276,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -7187,23 +7287,48 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>30</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>13:57:31</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>15:22</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D32" t="n">
-        <v>99</v>
-      </c>
-      <c r="E32" t="inlineStr">
+      <c r="D33" t="n">
+        <v>85</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 977
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E215"/>
+  <dimension ref="A1:E221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:57:31</t>
+          <t>Última actualización: 14:15:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 210</t>
+          <t>Total filas: 216</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5128,21 +5128,21 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5153,12 +5153,12 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -5167,7 +5167,7 @@
         </is>
       </c>
       <c r="D193" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,12 +5203,12 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>14:18</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -5217,7 +5217,7 @@
         </is>
       </c>
       <c r="D195" t="n">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5228,21 +5228,21 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:18</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5253,21 +5253,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>14:31</t>
+          <t>14:19</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5278,21 +5278,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>14:32</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5303,21 +5303,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:31</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,21 +5328,21 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:32</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5353,21 +5353,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,21 +5378,21 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5403,21 +5403,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>14:39</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5428,21 +5428,21 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>14:47</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5453,21 +5453,21 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5478,21 +5478,21 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5503,21 +5503,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,21 +5528,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>15:11</t>
+          <t>14:54</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,21 +5553,21 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5578,12 +5578,12 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:11</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -5592,7 +5592,7 @@
         </is>
       </c>
       <c r="D210" t="n">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,21 +5603,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5628,21 +5628,21 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>15:41</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,21 +5653,21 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,21 +5678,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5703,23 +5703,173 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>15:41</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>86</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>98</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>98</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>98</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
           <t>13:57:31</t>
         </is>
       </c>
-      <c r="B215" t="inlineStr">
+      <c r="B219" t="inlineStr">
         <is>
           <t>15:56</t>
         </is>
       </c>
-      <c r="C215" t="inlineStr">
+      <c r="C219" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D215" t="n">
+      <c r="D219" t="n">
         <v>119</v>
       </c>
-      <c r="E215" t="inlineStr">
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D220" t="n">
+        <v>102</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>110</v>
+      </c>
+      <c r="E221" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5754,7 +5904,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:57:31</t>
+          <t>Última actualización: 14:15:21</t>
         </is>
       </c>
     </row>
@@ -6445,7 +6595,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -6459,7 +6609,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -6470,7 +6620,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -6484,7 +6634,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -6520,7 +6670,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -6534,7 +6684,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -6545,7 +6695,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -6559,7 +6709,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -6578,7 +6728,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6596,14 +6746,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:57:31</t>
+          <t>Última actualización: 14:15:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -7287,7 +7437,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -7301,7 +7451,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -7312,7 +7462,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -7326,11 +7476,36 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16:02</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>107</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 978
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E221"/>
+  <dimension ref="A1:E226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:15:21</t>
+          <t>Última actualización: 14:33:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 216</t>
+          <t>Total filas: 221</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5353,7 +5353,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -5367,7 +5367,7 @@
         </is>
       </c>
       <c r="D201" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,21 +5378,21 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5408,16 +5408,16 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5428,21 +5428,21 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>14:39</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5453,21 +5453,21 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>14:47</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5478,7 +5478,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -5488,11 +5488,11 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5503,21 +5503,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,12 +5528,12 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -5542,7 +5542,7 @@
         </is>
       </c>
       <c r="D208" t="n">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5558,16 +5558,16 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:54</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5578,21 +5578,21 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>15:11</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>117</v>
+        <v>29</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,21 +5603,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:11</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5628,21 +5628,21 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,21 +5653,21 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:16</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,21 +5678,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5703,21 +5703,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>15:41</t>
+          <t>15:33</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5733,16 +5733,16 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5753,21 +5753,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5778,21 +5778,21 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:41</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5803,12 +5803,12 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:52</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -5817,7 +5817,7 @@
         </is>
       </c>
       <c r="D219" t="n">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5828,21 +5828,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>15:57</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5853,23 +5853,148 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>80</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>80</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>13:57:31</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>119</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
           <t>14:15:21</t>
         </is>
       </c>
-      <c r="B221" t="inlineStr">
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>102</v>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
         <is>
           <t>16:05</t>
         </is>
       </c>
-      <c r="C221" t="inlineStr">
+      <c r="C225" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D221" t="n">
-        <v>110</v>
-      </c>
-      <c r="E221" t="inlineStr">
+      <c r="D225" t="n">
+        <v>92</v>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>101</v>
+      </c>
+      <c r="E226" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5886,7 +6011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5904,14 +6029,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:15:21</t>
+          <t>Última actualización: 14:33:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 31</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -6570,7 +6695,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -6584,7 +6709,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -6620,7 +6745,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -6634,7 +6759,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -6645,7 +6770,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -6659,7 +6784,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -6695,23 +6820,48 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>60</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>14:15:21</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B37" t="inlineStr">
         <is>
           <t>15:34</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D36" t="n">
+      <c r="D37" t="n">
         <v>79</v>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6728,7 +6878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6746,14 +6896,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:15:21</t>
+          <t>Última actualización: 14:33:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
@@ -7462,50 +7612,150 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>15:22</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>48</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>14:15:21</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>15:22</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>67</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>88</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>16:02</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D37" t="n">
         <v>107</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>116</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 979
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E226"/>
+  <dimension ref="A1:E237"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:33:43</t>
+          <t>Última actualización: 14:47:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 221</t>
+          <t>Total filas: 232</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,7 +5203,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5213,11 +5213,11 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5478,21 +5478,21 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>14:48</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5517,7 +5517,7 @@
         </is>
       </c>
       <c r="D207" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5533,16 +5533,16 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,21 +5553,21 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:52</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5583,16 +5583,16 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,21 +5603,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>15:11</t>
+          <t>14:54</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5633,16 +5633,16 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,21 +5653,21 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>15:16</t>
+          <t>15:11</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,21 +5678,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5703,21 +5703,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>15:33</t>
+          <t>15:16</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5728,21 +5728,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5753,21 +5753,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:18</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5783,16 +5783,16 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>15:41</t>
+          <t>15:33</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5803,21 +5803,21 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>15:52</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5833,16 +5833,16 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5858,16 +5858,16 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:41</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5878,21 +5878,21 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:42</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5903,12 +5903,12 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:52</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -5917,7 +5917,7 @@
         </is>
       </c>
       <c r="D223" t="n">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,21 +5928,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>15:57</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,21 +5953,21 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>16:05</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,23 +5978,298 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>66</v>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>66</v>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>13:57:31</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>119</v>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>102</v>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
           <t>14:33:43</t>
         </is>
       </c>
-      <c r="B226" t="inlineStr">
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>92</v>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>16:06</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>79</v>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
         <is>
           <t>16:14</t>
         </is>
       </c>
-      <c r="C226" t="inlineStr">
+      <c r="C232" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D226" t="n">
-        <v>101</v>
-      </c>
-      <c r="E226" t="inlineStr">
+      <c r="D232" t="n">
+        <v>87</v>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>16:17</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>90</v>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>16:22</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>95</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>83_ALUAR</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>107</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>114</v>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>16:46</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>119</v>
+      </c>
+      <c r="E237" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6006,873 +6281,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - LP1912-215 - 25/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 14:33:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 32</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>05:58:04</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>06:16</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>18</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>06:38:54</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>06:56</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>18</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>06:56:24</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>06:57</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>07:15:48</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>07:15</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>06:56:24</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>07:16</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>07:15:48</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>07:43</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>28</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>07:40:11</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>07:44</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>08:40:59</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>08:43</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>3</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>08:30:14</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>08:44</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>14</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>08:53</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>08:30:14</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>08:54</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>24</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>08:40:59</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>08:57</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>17</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>08:58</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>6</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>09:23:52</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>09:58</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>35</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>09:59</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>67</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>10:41:48</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>49</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>11:13:01</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>11:31</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>18</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>11:35:40</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>11:41</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>6</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>11:13:01</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>11:42</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>29</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>11:35:40</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>12:21</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>46</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>12:12:04</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>12:22</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>10</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>12:54:41</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>13:03</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>9</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>12:47:00</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>13:04</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>17</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>12:33:54</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>13:32</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>59</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>13:14:41</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>13:33</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>19</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>14:33:43</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>14:33</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>14:15:21</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>14:34</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>19</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>14:33:43</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>14:47</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>14</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>14:33:43</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>14:53</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>215_EL PELIGRO</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>20</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>14:15:21</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>14:54</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>215_EL PELIGRO</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>39</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>14:33:43</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>15:33</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>60</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>14:15:21</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>15:34</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>79</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6889,14 +6297,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173 - 25/01/2026</t>
+          <t>LÍNEA 141 - LP1912-215 - 25/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:33:43</t>
+          <t>Última actualización: 14:47:05</t>
         </is>
       </c>
     </row>
@@ -6937,6 +6345,898 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>28</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:44</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>14</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>24</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>17</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>35</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>67</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>49</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>11:13:01</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>18</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>6</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>11:13:01</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>29</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>46</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>12:54:41</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>9</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>17</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>59</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>13:14:41</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>19</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>19</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>14</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:48</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>20</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>7</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>60</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>47</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - 6203-6173 - 25/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 14:47:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 34</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>07:15:48</t>
         </is>
       </c>
@@ -7662,7 +7962,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -7676,7 +7976,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -7712,7 +8012,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7726,7 +8026,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -7754,6 +8054,31 @@
         <v>116</v>
       </c>
       <c r="E38" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>103</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 980
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E237"/>
+  <dimension ref="A1:E247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:47:05</t>
+          <t>Última actualización: 14:53:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 232</t>
+          <t>Total filas: 242</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5578,7 +5578,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5592,7 +5592,7 @@
         </is>
       </c>
       <c r="D210" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5692,7 +5692,7 @@
         </is>
       </c>
       <c r="D214" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5703,7 +5703,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -5717,7 +5717,7 @@
         </is>
       </c>
       <c r="D215" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5728,7 +5728,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -5742,7 +5742,7 @@
         </is>
       </c>
       <c r="D216" t="n">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5778,7 +5778,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -5792,7 +5792,7 @@
         </is>
       </c>
       <c r="D218" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5828,7 +5828,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -5842,7 +5842,7 @@
         </is>
       </c>
       <c r="D220" t="n">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5853,7 +5853,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -5867,7 +5867,7 @@
         </is>
       </c>
       <c r="D221" t="n">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,21 +5928,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:52</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,21 +5953,21 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:52</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,12 +5978,12 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:52</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -5992,7 +5992,7 @@
         </is>
       </c>
       <c r="D226" t="n">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6028,21 +6028,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,12 +6053,12 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>15:57</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -6067,7 +6067,7 @@
         </is>
       </c>
       <c r="D229" t="n">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,21 +6078,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>16:05</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,21 +6103,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>16:06</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6128,21 +6128,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6153,21 +6153,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:04</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6178,21 +6178,21 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>16:22</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6208,16 +6208,16 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:06</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6228,21 +6228,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6258,18 +6258,268 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>87</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>14:53:58</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>16:16</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>83</v>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>16:17</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>90</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>14:53:58</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>88</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>16:22</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>95</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>14:53:58</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>83_ALUAR</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>100</v>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>83_ALUAR</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>107</v>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>14:53:58</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>107</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D245" t="n">
+        <v>114</v>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>14:53:58</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>16:45</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D246" t="n">
+        <v>112</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
           <t>16:46</t>
         </is>
       </c>
-      <c r="C237" t="inlineStr">
+      <c r="C247" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D237" t="n">
+      <c r="D247" t="n">
         <v>119</v>
       </c>
-      <c r="E237" t="inlineStr">
+      <c r="E247" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6304,7 +6554,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:47:05</t>
+          <t>Última actualización: 14:53:58</t>
         </is>
       </c>
     </row>
@@ -7070,7 +7320,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -7084,7 +7334,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -7120,7 +7370,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7134,7 +7384,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -7196,7 +7446,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:47:05</t>
+          <t>Última actualización: 14:53:58</t>
         </is>
       </c>
     </row>
@@ -7937,7 +8187,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -7951,7 +8201,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -7987,7 +8237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -8001,7 +8251,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -8037,7 +8287,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -8051,7 +8301,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 981
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E247"/>
+  <dimension ref="A1:E253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:53:58</t>
+          <t>Última actualización: 15:17:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 242</t>
+          <t>Total filas: 248</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,7 +5203,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5213,11 +5213,11 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5728,7 +5728,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -5742,7 +5742,7 @@
         </is>
       </c>
       <c r="D216" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5778,7 +5778,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -5792,7 +5792,7 @@
         </is>
       </c>
       <c r="D218" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5828,7 +5828,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -5842,7 +5842,7 @@
         </is>
       </c>
       <c r="D220" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5853,7 +5853,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -5867,7 +5867,7 @@
         </is>
       </c>
       <c r="D221" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5963,7 +5963,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D225" t="n">
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6042,7 +6042,7 @@
         </is>
       </c>
       <c r="D228" t="n">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6103,7 +6103,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6117,7 +6117,7 @@
         </is>
       </c>
       <c r="D231" t="n">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6178,7 +6178,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -6192,7 +6192,7 @@
         </is>
       </c>
       <c r="D234" t="n">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6203,21 +6203,21 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>16:06</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6228,21 +6228,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>16:13</t>
+          <t>16:06</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6253,12 +6253,12 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -6267,7 +6267,7 @@
         </is>
       </c>
       <c r="D237" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6278,21 +6278,21 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>16:16</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,12 +6303,12 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -6317,7 +6317,7 @@
         </is>
       </c>
       <c r="D239" t="n">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,21 +6328,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:17</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,12 +6353,12 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>16:22</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -6367,7 +6367,7 @@
         </is>
       </c>
       <c r="D241" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,21 +6378,21 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,21 +6403,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6433,16 +6433,16 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,21 +6453,21 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6478,21 +6478,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6508,18 +6508,168 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D247" t="n">
+        <v>114</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>14:53:58</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>16:45</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>112</v>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>15:17:56</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
           <t>16:46</t>
         </is>
       </c>
-      <c r="C247" t="inlineStr">
+      <c r="C249" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D247" t="n">
-        <v>119</v>
-      </c>
-      <c r="E247" t="inlineStr">
+      <c r="D249" t="n">
+        <v>89</v>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>15:17:56</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>96</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>15:17:56</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>16:58</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>101</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>15:17:56</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>110</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>15:17:56</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>17:09</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>112</v>
+      </c>
+      <c r="E253" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6531,898 +6681,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - LP1912-215 - 25/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 14:53:58</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 33</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>05:58:04</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>06:16</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>18</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>06:38:54</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>06:56</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>18</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>06:56:24</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>06:57</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>07:15:48</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>07:15</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>06:56:24</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>07:16</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>20</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>07:15:48</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>07:43</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>28</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>07:40:11</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>07:44</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>08:40:59</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>08:43</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>3</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>08:30:14</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>08:44</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>14</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>08:53</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>08:30:14</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>08:54</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>24</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>08:40:59</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>08:57</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>17</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>08:58</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>6</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>09:23:52</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>09:58</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>35</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>08:52:33</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>09:59</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>67</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>10:41:48</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>49</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>11:13:01</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>11:31</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>18</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>11:35:40</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>11:41</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>6</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>11:13:01</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>11:42</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>29</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>11:35:40</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>12:21</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>46</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>12:12:04</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>12:22</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>10</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>12:54:41</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>13:03</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>9</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>12:47:00</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>13:04</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>17</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>12:33:54</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>13:32</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>59</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>13:14:41</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>13:33</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>19</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>14:33:43</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>14:33</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>14:15:21</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>14:34</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>19</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>14:33:43</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>14:47</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>14</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>14:47:05</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>14:48</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>14:53:58</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>14:53</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>215_EL PELIGRO</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>14:47:05</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>14:54</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>215_EL PELIGRO</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>7</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>14:53:58</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>15:33</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>40</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>14:47:05</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>15:34</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>47</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -7439,14 +6697,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173 - 25/01/2026</t>
+          <t>LÍNEA 141 - LP1912-215 - 25/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:53:58</t>
+          <t>Última actualización: 15:17:56</t>
         </is>
       </c>
     </row>
@@ -7487,6 +6745,923 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>05:58:04</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06:38:54</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:56:24</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>07:15:48</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>28</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>07:40:11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:44</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>14</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:30:14</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>24</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>08:40:59</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>17</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>09:23:52</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>35</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:52:33</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>67</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>10:41:48</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>49</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>11:13:01</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>18</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>6</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>11:13:01</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>29</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>11:35:40</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>46</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>12:12:04</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>12:54:41</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>9</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12:47:00</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>17</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>59</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>13:14:41</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>19</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14:15:21</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>19</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14:33:43</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>14</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:48</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>14:53:58</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>7</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>15:17:56</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>16</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>14:47:05</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>47</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>15:17:56</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>17:09</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>112</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - 6203-6173 - 25/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 15:17:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 35</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>07:15:48</t>
         </is>
       </c>
@@ -8187,7 +8362,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -8201,7 +8376,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -8237,7 +8412,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -8251,7 +8426,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -8287,7 +8462,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -8301,7 +8476,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -8331,6 +8506,31 @@
       <c r="E39" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>15:17:56</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>108</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 982
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E253"/>
+  <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:17:56</t>
+          <t>Última actualización: 15:47:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 248</t>
+          <t>Total filas: 255</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6042,7 +6042,7 @@
         </is>
       </c>
       <c r="D228" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6067,7 +6067,7 @@
         </is>
       </c>
       <c r="D229" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6092,7 +6092,7 @@
         </is>
       </c>
       <c r="D230" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,7 +6103,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6117,7 +6117,7 @@
         </is>
       </c>
       <c r="D231" t="n">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6178,7 +6178,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -6192,7 +6192,7 @@
         </is>
       </c>
       <c r="D234" t="n">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6203,7 +6203,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -6217,7 +6217,7 @@
         </is>
       </c>
       <c r="D235" t="n">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6278,7 +6278,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -6292,7 +6292,7 @@
         </is>
       </c>
       <c r="D238" t="n">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6328,7 +6328,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -6342,7 +6342,7 @@
         </is>
       </c>
       <c r="D240" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6367,7 +6367,7 @@
         </is>
       </c>
       <c r="D241" t="n">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6403,21 +6403,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,21 +6428,21 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,12 +6453,12 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -6467,7 +6467,7 @@
         </is>
       </c>
       <c r="D245" t="n">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6478,21 +6478,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6503,12 +6503,12 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -6517,7 +6517,7 @@
         </is>
       </c>
       <c r="D247" t="n">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6528,21 +6528,21 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6553,12 +6553,12 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>16:46</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -6567,7 +6567,7 @@
         </is>
       </c>
       <c r="D249" t="n">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6583,16 +6583,16 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:46</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6603,21 +6603,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6628,21 +6628,21 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>110</v>
+        <v>71</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6653,23 +6653,198 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>80</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>80</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
           <t>17:09</t>
         </is>
       </c>
-      <c r="C253" t="inlineStr">
+      <c r="C255" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D253" t="n">
-        <v>112</v>
-      </c>
-      <c r="E253" t="inlineStr">
+      <c r="D255" t="n">
+        <v>82</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>94</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>107</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>109</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>111</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>115</v>
+      </c>
+      <c r="E260" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6686,7 +6861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6704,14 +6879,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:17:56</t>
+          <t>Última actualización: 15:47:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 34</t>
+          <t>Total filas: 36</t>
         </is>
       </c>
     </row>
@@ -7570,7 +7745,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -7584,9 +7759,59 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>111</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>115</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7621,7 +7846,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:17:56</t>
+          <t>Última actualización: 15:47:48</t>
         </is>
       </c>
     </row>
@@ -8412,7 +8637,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -8426,7 +8651,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -8462,7 +8687,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -8476,7 +8701,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -8512,7 +8737,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -8526,7 +8751,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 983
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E260"/>
+  <dimension ref="A1:E265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:47:48</t>
+          <t>Última actualización: 15:59:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 255</t>
+          <t>Total filas: 260</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5963,7 +5963,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D225" t="n">
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6003,7 +6003,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6013,11 +6013,11 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6178,7 +6178,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -6192,7 +6192,7 @@
         </is>
       </c>
       <c r="D234" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6203,7 +6203,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -6217,7 +6217,7 @@
         </is>
       </c>
       <c r="D235" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6278,7 +6278,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -6292,7 +6292,7 @@
         </is>
       </c>
       <c r="D238" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6328,7 +6328,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -6342,7 +6342,7 @@
         </is>
       </c>
       <c r="D240" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6367,7 +6367,7 @@
         </is>
       </c>
       <c r="D241" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6417,7 +6417,7 @@
         </is>
       </c>
       <c r="D243" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6478,7 +6478,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -6492,7 +6492,7 @@
         </is>
       </c>
       <c r="D246" t="n">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6528,7 +6528,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -6542,7 +6542,7 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6603,7 +6603,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6617,7 +6617,7 @@
         </is>
       </c>
       <c r="D251" t="n">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6628,21 +6628,21 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6653,21 +6653,21 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6678,21 +6678,21 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:06</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6708,16 +6708,16 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6728,21 +6728,21 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6753,21 +6753,21 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:08</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,21 +6778,21 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>109</v>
+        <v>70</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6803,21 +6803,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6828,23 +6828,148 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
+          <t>15:59:49</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>17:33</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>94</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>15:59:49</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>95</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
           <t>15:47:47</t>
         </is>
       </c>
-      <c r="B260" t="inlineStr">
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>109</v>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>15:59:49</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>99</v>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
         <is>
           <t>17:42</t>
         </is>
       </c>
-      <c r="C260" t="inlineStr">
+      <c r="C264" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D260" t="n">
+      <c r="D264" t="n">
         <v>115</v>
       </c>
-      <c r="E260" t="inlineStr">
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>15:59:49</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>106</v>
+      </c>
+      <c r="E265" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6861,7 +6986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6879,14 +7004,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:47:48</t>
+          <t>Última actualización: 15:59:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 36</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
     </row>
@@ -7745,7 +7870,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -7759,7 +7884,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -7770,7 +7895,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -7784,7 +7909,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -7812,6 +7937,31 @@
         <v>115</v>
       </c>
       <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>15:59:49</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>106</v>
+      </c>
+      <c r="E42" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7846,7 +7996,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:47:48</t>
+          <t>Última actualización: 15:59:49</t>
         </is>
       </c>
     </row>
@@ -8637,7 +8787,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -8651,7 +8801,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -8687,7 +8837,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -8701,7 +8851,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -8737,7 +8887,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -8751,7 +8901,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 984
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E265"/>
+  <dimension ref="A1:E275"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:59:49</t>
+          <t>Última actualización: 16:19:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 260</t>
+          <t>Total filas: 270</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6367,7 +6367,7 @@
         </is>
       </c>
       <c r="D241" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6417,7 +6417,7 @@
         </is>
       </c>
       <c r="D243" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6442,7 +6442,7 @@
         </is>
       </c>
       <c r="D244" t="n">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6478,7 +6478,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -6492,7 +6492,7 @@
         </is>
       </c>
       <c r="D246" t="n">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6528,7 +6528,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -6542,7 +6542,7 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6603,7 +6603,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6617,7 +6617,7 @@
         </is>
       </c>
       <c r="D251" t="n">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6628,7 +6628,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -6642,7 +6642,7 @@
         </is>
       </c>
       <c r="D252" t="n">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6653,7 +6653,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -6667,7 +6667,7 @@
         </is>
       </c>
       <c r="D253" t="n">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6678,12 +6678,12 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>17:06</t>
+          <t>17:01</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -6692,7 +6692,7 @@
         </is>
       </c>
       <c r="D254" t="n">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6703,12 +6703,12 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:06</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -6717,7 +6717,7 @@
         </is>
       </c>
       <c r="D255" t="n">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6728,7 +6728,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -6742,7 +6742,7 @@
         </is>
       </c>
       <c r="D256" t="n">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6753,21 +6753,21 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>17:08</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6783,16 +6783,16 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:08</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6808,16 +6808,16 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6828,21 +6828,21 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6853,21 +6853,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,12 +6878,12 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -6892,7 +6892,7 @@
         </is>
       </c>
       <c r="D262" t="n">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6908,16 +6908,16 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,21 +6928,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,23 +6953,273 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>109</v>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>16:19:28</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>79</v>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>115</v>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
           <t>15:59:49</t>
         </is>
       </c>
-      <c r="B265" t="inlineStr">
+      <c r="B268" t="inlineStr">
         <is>
           <t>17:45</t>
         </is>
       </c>
-      <c r="C265" t="inlineStr">
+      <c r="C268" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D265" t="n">
+      <c r="D268" t="n">
         <v>106</v>
       </c>
-      <c r="E265" t="inlineStr">
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>16:19:28</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>87</v>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>16:19:28</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>17:53</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>94</v>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>16:19:28</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>17:58</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>99</v>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>16:19:28</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>106</v>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>16:19:28</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>111</v>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>16:19:28</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>111</v>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>16:19:28</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>18:17</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>118</v>
+      </c>
+      <c r="E275" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6986,7 +7236,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7004,14 +7254,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:59:49</t>
+          <t>Última actualización: 16:19:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 39</t>
         </is>
       </c>
     </row>
@@ -7895,21 +8145,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -7920,21 +8170,21 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -7945,23 +8195,73 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>15:47:47</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>115</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>15:59:49</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B43" t="inlineStr">
         <is>
           <t>17:45</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D42" t="n">
+      <c r="D43" t="n">
         <v>106</v>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>16:19:28</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>87</v>
+      </c>
+      <c r="E44" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7978,7 +8278,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7996,14 +8296,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:59:49</t>
+          <t>Última actualización: 16:19:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 36</t>
         </is>
       </c>
     </row>
@@ -8362,7 +8662,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -8372,11 +8672,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -8387,7 +8687,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -8397,11 +8697,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -8862,7 +9162,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -8876,7 +9176,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -8904,6 +9204,31 @@
         <v>66</v>
       </c>
       <c r="E40" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>16:19:28</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>17:06</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>47</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 985
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E275"/>
+  <dimension ref="A1:E280"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:19:29</t>
+          <t>Última actualización: 16:31:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 270</t>
+          <t>Total filas: 275</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,7 +5203,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5213,11 +5213,11 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6478,7 +6478,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -6492,7 +6492,7 @@
         </is>
       </c>
       <c r="D246" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6528,7 +6528,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -6542,7 +6542,7 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6603,7 +6603,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6617,7 +6617,7 @@
         </is>
       </c>
       <c r="D251" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6628,7 +6628,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -6642,7 +6642,7 @@
         </is>
       </c>
       <c r="D252" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6653,7 +6653,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -6667,7 +6667,7 @@
         </is>
       </c>
       <c r="D253" t="n">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6703,7 +6703,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -6717,7 +6717,7 @@
         </is>
       </c>
       <c r="D255" t="n">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6728,7 +6728,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -6738,11 +6738,11 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6803,7 +6803,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -6817,7 +6817,7 @@
         </is>
       </c>
       <c r="D259" t="n">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6853,7 +6853,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6867,7 +6867,7 @@
         </is>
       </c>
       <c r="D261" t="n">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,7 +6878,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -6892,7 +6892,7 @@
         </is>
       </c>
       <c r="D262" t="n">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6928,7 +6928,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -6942,7 +6942,7 @@
         </is>
       </c>
       <c r="D264" t="n">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6978,7 +6978,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -6992,7 +6992,7 @@
         </is>
       </c>
       <c r="D266" t="n">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7028,7 +7028,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -7042,7 +7042,7 @@
         </is>
       </c>
       <c r="D268" t="n">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7078,12 +7078,12 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -7092,7 +7092,7 @@
         </is>
       </c>
       <c r="D270" t="n">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,21 +7103,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7133,16 +7133,16 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7153,21 +7153,21 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7178,21 +7178,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7203,23 +7203,148 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>99</v>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>16:31:43</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>99</v>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>16:31:43</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
           <t>18:17</t>
         </is>
       </c>
-      <c r="C275" t="inlineStr">
+      <c r="C277" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D275" t="n">
+      <c r="D277" t="n">
+        <v>106</v>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>16:31:43</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>110</v>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>16:31:43</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>114</v>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>16:31:43</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>18:29</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
         <v>118</v>
       </c>
-      <c r="E275" t="inlineStr">
+      <c r="E280" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7236,7 +7361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7254,14 +7379,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:19:29</t>
+          <t>Última actualización: 16:31:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 39</t>
+          <t>Total filas: 40</t>
         </is>
       </c>
     </row>
@@ -8120,7 +8245,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -8134,7 +8259,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -8170,7 +8295,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -8184,7 +8309,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -8220,7 +8345,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -8234,7 +8359,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -8262,6 +8387,31 @@
         <v>87</v>
       </c>
       <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>16:31:43</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>110</v>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8278,7 +8428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8296,14 +8446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:19:29</t>
+          <t>Última actualización: 16:31:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 36</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
     </row>
@@ -9187,48 +9337,73 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>16:31</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>16:31:43</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>34</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>16:19:28</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>17:06</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="D42" t="n">
         <v>47</v>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 986
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E280"/>
+  <dimension ref="A1:E289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:31:43</t>
+          <t>Última actualización: 16:44:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 275</t>
+          <t>Total filas: 284</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6628,21 +6628,21 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>16:54</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6653,21 +6653,21 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6678,21 +6678,21 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>17:01</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6703,12 +6703,12 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>17:06</t>
+          <t>17:01</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -6717,7 +6717,7 @@
         </is>
       </c>
       <c r="D255" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6728,12 +6728,12 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:06</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -6742,7 +6742,7 @@
         </is>
       </c>
       <c r="D256" t="n">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6767,7 +6767,7 @@
         </is>
       </c>
       <c r="D257" t="n">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,21 +6778,21 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>17:08</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6803,21 +6803,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:08</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6828,12 +6828,12 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -6842,7 +6842,7 @@
         </is>
       </c>
       <c r="D260" t="n">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6853,21 +6853,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,21 +6878,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6903,12 +6903,12 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>15:59:49</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -6917,7 +6917,7 @@
         </is>
       </c>
       <c r="D263" t="n">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,21 +6928,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>15:59:49</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,21 +6953,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6978,21 +6978,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7003,21 +7003,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7033,16 +7033,16 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7053,21 +7053,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7078,21 +7078,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:42</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7108,16 +7108,16 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7128,21 +7128,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7158,16 +7158,16 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7178,21 +7178,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7208,16 +7208,16 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,21 +7228,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7253,12 +7253,12 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:19:28</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -7267,7 +7267,7 @@
         </is>
       </c>
       <c r="D277" t="n">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,21 +7278,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7308,16 +7308,16 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7328,23 +7328,248 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>18:06</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>82</v>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>86</v>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>86</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>18:17</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>93</v>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
           <t>16:31:43</t>
         </is>
       </c>
-      <c r="B280" t="inlineStr">
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>110</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>98</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>101</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>16:31:43</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
         <is>
           <t>18:29</t>
         </is>
       </c>
-      <c r="C280" t="inlineStr">
+      <c r="C287" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D280" t="n">
+      <c r="D287" t="n">
         <v>118</v>
       </c>
-      <c r="E280" t="inlineStr">
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>106</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>112</v>
+      </c>
+      <c r="E289" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7361,7 +7586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7379,14 +7604,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:31:43</t>
+          <t>Última actualización: 16:44:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 40</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -8270,7 +8495,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -8284,7 +8509,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -8320,21 +8545,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>115</v>
+        <v>55</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -8345,12 +8570,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:42</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -8359,7 +8584,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -8370,12 +8595,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -8384,7 +8609,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -8395,23 +8620,73 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>62</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>16:31:43</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B46" t="inlineStr">
         <is>
           <t>18:21</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="D46" t="n">
         <v>110</v>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>98</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8428,7 +8703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8446,14 +8721,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:31:43</t>
+          <t>Última actualización: 16:44:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -8812,7 +9087,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -8822,11 +9097,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -8837,7 +9112,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -8847,11 +9122,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -9387,7 +9662,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -9401,9 +9676,34 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E42" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>16:44:07</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>112</v>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 987
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E289"/>
+  <dimension ref="A1:E290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:44:07</t>
+          <t>Última actualización: 16:52:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 284</t>
+          <t>Total filas: 285</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6038,7 +6038,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6603,7 +6603,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6617,7 +6617,7 @@
         </is>
       </c>
       <c r="D251" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6653,7 +6653,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -6667,7 +6667,7 @@
         </is>
       </c>
       <c r="D253" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6678,7 +6678,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -6692,7 +6692,7 @@
         </is>
       </c>
       <c r="D254" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6728,7 +6728,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -6742,7 +6742,7 @@
         </is>
       </c>
       <c r="D256" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6767,7 +6767,7 @@
         </is>
       </c>
       <c r="D257" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6853,7 +6853,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6867,7 +6867,7 @@
         </is>
       </c>
       <c r="D261" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,7 +6878,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -6892,7 +6892,7 @@
         </is>
       </c>
       <c r="D262" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6953,7 +6953,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -6967,7 +6967,7 @@
         </is>
       </c>
       <c r="D265" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6978,7 +6978,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -6992,7 +6992,7 @@
         </is>
       </c>
       <c r="D266" t="n">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7028,7 +7028,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -7042,7 +7042,7 @@
         </is>
       </c>
       <c r="D268" t="n">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7128,7 +7128,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -7142,7 +7142,7 @@
         </is>
       </c>
       <c r="D272" t="n">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7203,12 +7203,12 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -7217,7 +7217,7 @@
         </is>
       </c>
       <c r="D275" t="n">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,12 +7228,12 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -7242,7 +7242,7 @@
         </is>
       </c>
       <c r="D276" t="n">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>16:19:28</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,21 +7278,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,21 +7303,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7328,12 +7328,12 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -7342,7 +7342,7 @@
         </is>
       </c>
       <c r="D280" t="n">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7358,16 +7358,16 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7392,7 +7392,7 @@
         </is>
       </c>
       <c r="D282" t="n">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,21 +7403,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,21 +7428,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7453,12 +7453,12 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -7467,7 +7467,7 @@
         </is>
       </c>
       <c r="D285" t="n">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7478,21 +7478,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,21 +7503,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>18:29</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7528,12 +7528,12 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:29</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -7542,7 +7542,7 @@
         </is>
       </c>
       <c r="D288" t="n">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7558,18 +7558,43 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>106</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>16:52:32</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
           <t>18:36</t>
         </is>
       </c>
-      <c r="C289" t="inlineStr">
+      <c r="C290" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D289" t="n">
-        <v>112</v>
-      </c>
-      <c r="E289" t="inlineStr">
+      <c r="D290" t="n">
+        <v>104</v>
+      </c>
+      <c r="E290" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7604,7 +7629,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:44:07</t>
+          <t>Última actualización: 16:52:32</t>
         </is>
       </c>
     </row>
@@ -8495,7 +8520,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -8509,7 +8534,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -8520,7 +8545,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -8534,7 +8559,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -8620,7 +8645,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -8634,7 +8659,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -8670,7 +8695,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -8684,7 +8709,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -8721,7 +8746,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:44:07</t>
+          <t>Última actualización: 16:52:32</t>
         </is>
       </c>
     </row>
@@ -9662,7 +9687,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -9676,7 +9701,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -9687,7 +9712,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -9701,7 +9726,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 988
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E290"/>
+  <dimension ref="A1:E296"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:32</t>
+          <t>Última actualización: 17:14:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 285</t>
+          <t>Total filas: 291</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6878,7 +6878,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -6892,7 +6892,7 @@
         </is>
       </c>
       <c r="D262" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6953,7 +6953,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -6967,7 +6967,7 @@
         </is>
       </c>
       <c r="D265" t="n">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -7003,7 +7003,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -7017,7 +7017,7 @@
         </is>
       </c>
       <c r="D267" t="n">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7053,7 +7053,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -7067,7 +7067,7 @@
         </is>
       </c>
       <c r="D269" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7128,7 +7128,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -7142,7 +7142,7 @@
         </is>
       </c>
       <c r="D272" t="n">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7203,7 +7203,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -7217,7 +7217,7 @@
         </is>
       </c>
       <c r="D275" t="n">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7292,7 +7292,7 @@
         </is>
       </c>
       <c r="D278" t="n">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,7 +7303,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -7317,7 +7317,7 @@
         </is>
       </c>
       <c r="D279" t="n">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7367,7 +7367,7 @@
         </is>
       </c>
       <c r="D281" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7392,7 +7392,7 @@
         </is>
       </c>
       <c r="D282" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,7 +7403,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7417,7 +7417,7 @@
         </is>
       </c>
       <c r="D283" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7492,7 +7492,7 @@
         </is>
       </c>
       <c r="D286" t="n">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7517,7 +7517,7 @@
         </is>
       </c>
       <c r="D287" t="n">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7567,7 +7567,7 @@
         </is>
       </c>
       <c r="D289" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7592,9 +7592,159 @@
         </is>
       </c>
       <c r="D290" t="n">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="E290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>17:14:15</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D291" t="n">
+        <v>82</v>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>17:14:15</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>87</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>17:14:15</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>91</v>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>17:14:15</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>18:57</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>103</v>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>17:14:15</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>106</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>17:14:15</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>110</v>
+      </c>
+      <c r="E296" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7611,7 +7761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7629,14 +7779,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:32</t>
+          <t>Última actualización: 17:14:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 43</t>
         </is>
       </c>
     </row>
@@ -8570,7 +8720,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -8584,7 +8734,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -8645,7 +8795,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -8659,7 +8809,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -8695,7 +8845,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -8709,9 +8859,34 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>17:14:15</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>110</v>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8746,7 +8921,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:32</t>
+          <t>Última actualización: 17:14:16</t>
         </is>
       </c>
     </row>
@@ -9712,7 +9887,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -9726,7 +9901,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 989
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E296"/>
+  <dimension ref="A1:E302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:14:16</t>
+          <t>Última actualización: 17:38:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 291</t>
+          <t>Total filas: 297</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,7 +5203,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5213,11 +5213,11 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6038,7 +6038,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -7053,7 +7053,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -7067,7 +7067,7 @@
         </is>
       </c>
       <c r="D269" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7128,7 +7128,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -7142,7 +7142,7 @@
         </is>
       </c>
       <c r="D272" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7203,7 +7203,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -7217,7 +7217,7 @@
         </is>
       </c>
       <c r="D275" t="n">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7288,11 +7288,11 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,7 +7303,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -7317,7 +7317,7 @@
         </is>
       </c>
       <c r="D279" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7367,7 +7367,7 @@
         </is>
       </c>
       <c r="D281" t="n">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7392,7 +7392,7 @@
         </is>
       </c>
       <c r="D282" t="n">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,7 +7403,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7417,7 +7417,7 @@
         </is>
       </c>
       <c r="D283" t="n">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7492,7 +7492,7 @@
         </is>
       </c>
       <c r="D286" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7517,7 +7517,7 @@
         </is>
       </c>
       <c r="D287" t="n">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,21 +7578,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7603,7 +7603,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -7613,11 +7613,11 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7633,16 +7633,16 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,21 +7653,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,21 +7678,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,21 +7703,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,23 +7728,173 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
+          <t>18:57</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>79</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>17:38:13</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>82</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>17:38:13</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
           <t>19:04</t>
         </is>
       </c>
-      <c r="C296" t="inlineStr">
+      <c r="C298" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D296" t="n">
+      <c r="D298" t="n">
+        <v>86</v>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>17:38:13</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>99</v>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>17:38:13</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>99</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>17:38:13</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
         <v>110</v>
       </c>
-      <c r="E296" t="inlineStr">
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>17:38:13</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>19:36</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>118</v>
+      </c>
+      <c r="E302" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7761,7 +7911,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7779,14 +7929,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:14:16</t>
+          <t>Última actualización: 17:38:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 43</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -8720,7 +8870,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -8734,7 +8884,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -8795,7 +8945,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -8809,7 +8959,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -8845,7 +8995,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -8859,7 +9009,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -8870,7 +9020,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -8884,9 +9034,34 @@
         </is>
       </c>
       <c r="D48" t="n">
+        <v>86</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>17:38:13</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
         <v>110</v>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8903,7 +9078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8921,14 +9096,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:14:16</t>
+          <t>Última actualización: 17:38:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 39</t>
         </is>
       </c>
     </row>
@@ -9887,7 +10062,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -9901,11 +10076,36 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>17:38:13</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>19:24</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>106</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 990
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E302"/>
+  <dimension ref="A1:E307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:38:13</t>
+          <t>Última actualización: 17:51:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 297</t>
+          <t>Total filas: 302</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7288,11 +7288,11 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,21 +7303,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:54</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7328,21 +7328,21 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,12 +7353,12 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -7367,7 +7367,7 @@
         </is>
       </c>
       <c r="D281" t="n">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,21 +7378,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,7 +7403,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7413,11 +7413,11 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,21 +7428,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7453,21 +7453,21 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7478,12 +7478,12 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -7492,7 +7492,7 @@
         </is>
       </c>
       <c r="D286" t="n">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,21 +7503,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7528,21 +7528,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>18:29</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7553,21 +7553,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:29</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7588,7 +7588,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D290" t="n">
@@ -7603,21 +7603,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7628,12 +7628,12 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:33</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -7642,7 +7642,7 @@
         </is>
       </c>
       <c r="D292" t="n">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,21 +7653,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:14:15</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,21 +7678,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,21 +7703,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,21 +7728,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,21 +7753,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7778,21 +7778,21 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7803,21 +7803,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7828,21 +7828,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:13</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,23 +7878,148 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
+          <t>17:51:15</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>86</v>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
           <t>17:38:13</t>
         </is>
       </c>
-      <c r="B302" t="inlineStr">
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>99</v>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>17:51:15</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>97</v>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>17:51:15</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
         <is>
           <t>19:36</t>
         </is>
       </c>
-      <c r="C302" t="inlineStr">
+      <c r="C305" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D302" t="n">
-        <v>118</v>
-      </c>
-      <c r="E302" t="inlineStr">
+      <c r="D305" t="n">
+        <v>105</v>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>17:51:15</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>108</v>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>17:51:15</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>19:48</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>117</v>
+      </c>
+      <c r="E307" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7929,7 +8054,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:38:13</t>
+          <t>Última actualización: 17:51:15</t>
         </is>
       </c>
     </row>
@@ -8995,7 +9120,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -9009,7 +9134,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -9020,7 +9145,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -9034,7 +9159,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -9045,7 +9170,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -9059,7 +9184,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -9096,7 +9221,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:38:13</t>
+          <t>Última actualización: 17:51:15</t>
         </is>
       </c>
     </row>
@@ -10062,7 +10187,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -10076,7 +10201,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -10087,7 +10212,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -10101,7 +10226,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 991
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E307"/>
+  <dimension ref="A1:E316"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:51:15</t>
+          <t>Última actualización: 18:11:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 302</t>
+          <t>Total filas: 311</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,7 +5203,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5213,11 +5213,11 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7438,7 +7438,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -7453,21 +7453,21 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:11</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7478,21 +7478,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>16:31:43</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:11</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,21 +7503,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7528,21 +7528,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>16:31:43</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7553,21 +7553,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>18:29</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,21 +7578,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7603,12 +7603,12 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:29</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -7617,7 +7617,7 @@
         </is>
       </c>
       <c r="D291" t="n">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7633,16 +7633,16 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>18:33</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,12 +7653,12 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:14:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -7667,7 +7667,7 @@
         </is>
       </c>
       <c r="D293" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7683,16 +7683,16 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:33</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,21 +7703,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,21 +7728,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,21 +7753,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7778,21 +7778,21 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7803,21 +7803,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7828,21 +7828,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>19:13</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7883,16 +7883,16 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7903,21 +7903,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,21 +7928,21 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7953,21 +7953,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7983,16 +7983,16 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:13</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,23 +8003,248 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
+          <t>18:11:21</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>65</v>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>18:11:21</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>66</v>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>17:38:13</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>99</v>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>18:11:21</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>19:24</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>73</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>18:11:21</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>77</v>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>18:11:21</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>19:35</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>84</v>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
           <t>17:51:15</t>
         </is>
       </c>
-      <c r="B307" t="inlineStr">
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>19:36</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>105</v>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>18:11:21</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>88</v>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>18:11:21</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
         <is>
           <t>19:48</t>
         </is>
       </c>
-      <c r="C307" t="inlineStr">
+      <c r="C315" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D307" t="n">
-        <v>117</v>
-      </c>
-      <c r="E307" t="inlineStr">
+      <c r="D315" t="n">
+        <v>97</v>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>18:11:21</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>101</v>
+      </c>
+      <c r="E316" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8054,7 +8279,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:51:15</t>
+          <t>Última actualización: 18:11:21</t>
         </is>
       </c>
     </row>
@@ -9120,7 +9345,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -9134,7 +9359,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -9145,7 +9370,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -9159,7 +9384,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -9170,7 +9395,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -9184,7 +9409,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -9203,7 +9428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9221,14 +9446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:51:15</t>
+          <t>Última actualización: 18:11:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 39</t>
+          <t>Total filas: 40</t>
         </is>
       </c>
     </row>
@@ -10187,7 +10412,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -10201,7 +10426,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -10212,7 +10437,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -10226,11 +10451,36 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>18:11:21</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>19:58</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>107</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 992
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E316"/>
+  <dimension ref="A1:E322"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:11:21</t>
+          <t>Última actualización: 18:32:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 311</t>
+          <t>Total filas: 317</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7288,11 +7288,11 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7438,7 +7438,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -7463,7 +7463,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D285" t="n">
@@ -7488,7 +7488,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,7 +7728,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -7738,11 +7738,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,7 +7753,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7767,7 +7767,7 @@
         </is>
       </c>
       <c r="D297" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7778,7 +7778,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -7792,7 +7792,7 @@
         </is>
       </c>
       <c r="D298" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7803,7 +7803,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -7817,7 +7817,7 @@
         </is>
       </c>
       <c r="D299" t="n">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7828,7 +7828,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -7842,7 +7842,7 @@
         </is>
       </c>
       <c r="D300" t="n">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7867,7 +7867,7 @@
         </is>
       </c>
       <c r="D301" t="n">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7903,7 +7903,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -7917,7 +7917,7 @@
         </is>
       </c>
       <c r="D303" t="n">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,7 +7928,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -7942,7 +7942,7 @@
         </is>
       </c>
       <c r="D304" t="n">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8017,7 +8017,7 @@
         </is>
       </c>
       <c r="D307" t="n">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8042,7 +8042,7 @@
         </is>
       </c>
       <c r="D308" t="n">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8067,7 +8067,7 @@
         </is>
       </c>
       <c r="D309" t="n">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,12 +8078,12 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>19:24</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -8092,7 +8092,7 @@
         </is>
       </c>
       <c r="D310" t="n">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8108,16 +8108,16 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:24</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8128,21 +8128,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8153,12 +8153,12 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -8167,7 +8167,7 @@
         </is>
       </c>
       <c r="D313" t="n">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8178,21 +8178,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8203,21 +8203,21 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>19:48</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8233,18 +8233,168 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
+          <t>19:48</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>97</v>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>18:32:18</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
           <t>19:52</t>
         </is>
       </c>
-      <c r="C316" t="inlineStr">
+      <c r="C317" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D316" t="n">
-        <v>101</v>
-      </c>
-      <c r="E316" t="inlineStr">
+      <c r="D317" t="n">
+        <v>80</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>18:32:18</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>81</v>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>18:32:18</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>20:07</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>95</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>18:32:18</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>100</v>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>18:32:18</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>110</v>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>18:32:18</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>119</v>
+      </c>
+      <c r="E322" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8261,7 +8411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8279,14 +8429,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:11:21</t>
+          <t>Última actualización: 18:32:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -9370,7 +9520,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -9384,7 +9534,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -9395,7 +9545,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -9409,9 +9559,34 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>18:32:18</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>20:07</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>95</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9446,7 +9621,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:11:21</t>
+          <t>Última actualización: 18:32:18</t>
         </is>
       </c>
     </row>
@@ -10412,7 +10587,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -10426,7 +10601,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -10437,7 +10612,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -10451,7 +10626,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -10462,7 +10637,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -10476,7 +10651,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 993
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E322"/>
+  <dimension ref="A1:E327"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:32:18</t>
+          <t>Última actualización: 18:46:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 317</t>
+          <t>Total filas: 322</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7438,7 +7438,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -7803,21 +7803,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:46</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7828,21 +7828,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,12 +7878,12 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -7892,7 +7892,7 @@
         </is>
       </c>
       <c r="D302" t="n">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7903,21 +7903,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,21 +7928,21 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7953,21 +7953,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7978,12 +7978,12 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>19:13</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -7992,7 +7992,7 @@
         </is>
       </c>
       <c r="D306" t="n">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,21 +8003,21 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:13</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,21 +8028,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,21 +8078,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,12 +8103,12 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:32:18</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>19:24</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -8117,7 +8117,7 @@
         </is>
       </c>
       <c r="D311" t="n">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8128,21 +8128,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:22</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8153,21 +8153,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:24</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8178,21 +8178,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8208,16 +8208,16 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,21 +8228,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>19:48</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8253,21 +8253,21 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8278,12 +8278,12 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:48</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -8292,7 +8292,7 @@
         </is>
       </c>
       <c r="D318" t="n">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8303,21 +8303,21 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8328,21 +8328,21 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8353,21 +8353,21 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8378,23 +8378,148 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
+          <t>18:46:03</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>20:05</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>79</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>18:46:03</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>20:07</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>81</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
           <t>18:32:18</t>
         </is>
       </c>
-      <c r="B322" t="inlineStr">
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>100</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>18:46:03</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>20:13</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>87</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>18:46:03</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>96</v>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>18:46:03</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
         <is>
           <t>20:31</t>
         </is>
       </c>
-      <c r="C322" t="inlineStr">
+      <c r="C327" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D322" t="n">
-        <v>119</v>
-      </c>
-      <c r="E322" t="inlineStr">
+      <c r="D327" t="n">
+        <v>105</v>
+      </c>
+      <c r="E327" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8429,7 +8554,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:32:18</t>
+          <t>Última actualización: 18:46:03</t>
         </is>
       </c>
     </row>
@@ -9520,7 +9645,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -9534,7 +9659,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -9545,7 +9670,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -9559,7 +9684,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -9570,7 +9695,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -9584,7 +9709,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -9621,7 +9746,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:32:18</t>
+          <t>Última actualización: 18:46:03</t>
         </is>
       </c>
     </row>
@@ -10612,7 +10737,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -10626,7 +10751,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -10637,7 +10762,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -10651,7 +10776,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 994
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E327"/>
+  <dimension ref="A1:E332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:46:03</t>
+          <t>Última actualización: 18:52:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 322</t>
+          <t>Total filas: 327</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6003,7 +6003,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6013,11 +6013,11 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7288,11 +7288,11 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7438,7 +7438,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:54</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,21 +7878,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7903,12 +7903,12 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -7917,7 +7917,7 @@
         </is>
       </c>
       <c r="D303" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7933,16 +7933,16 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7953,21 +7953,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7978,21 +7978,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,12 +8003,12 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>19:13</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -8017,7 +8017,7 @@
         </is>
       </c>
       <c r="D307" t="n">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,21 +8028,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:13</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,21 +8053,21 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,21 +8078,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,21 +8103,21 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8133,16 +8133,16 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>19:22</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8153,12 +8153,12 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>19:24</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -8167,7 +8167,7 @@
         </is>
       </c>
       <c r="D313" t="n">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8183,16 +8183,16 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:22</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8203,21 +8203,21 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:24</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,21 +8228,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8253,21 +8253,21 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8278,21 +8278,21 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>19:48</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8303,21 +8303,21 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8328,21 +8328,21 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:48</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8353,21 +8353,21 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8378,21 +8378,21 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>20:05</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,21 +8403,21 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,21 +8428,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>18:32:18</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8458,16 +8458,16 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:05</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,21 +8478,21 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8503,23 +8503,148 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
+          <t>18:52:36</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>80</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
           <t>18:46:03</t>
         </is>
       </c>
-      <c r="B327" t="inlineStr">
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>20:13</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D328" t="n">
+        <v>87</v>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>18:52:36</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>90</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>18:52:36</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>98</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>18:46:03</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
         <is>
           <t>20:31</t>
         </is>
       </c>
-      <c r="C327" t="inlineStr">
+      <c r="C331" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D327" t="n">
+      <c r="D331" t="n">
         <v>105</v>
       </c>
-      <c r="E327" t="inlineStr">
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>18:52:36</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>20:47</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>115</v>
+      </c>
+      <c r="E332" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8536,7 +8661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8554,14 +8679,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:46:03</t>
+          <t>Última actualización: 18:52:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
     </row>
@@ -9645,7 +9770,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -9659,7 +9784,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -9670,7 +9795,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -9684,7 +9809,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -9695,7 +9820,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -9709,9 +9834,34 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>18:52:36</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>20:47</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>115</v>
+      </c>
+      <c r="E51" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9728,7 +9878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9746,14 +9896,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:46:03</t>
+          <t>Última actualización: 18:52:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 40</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -10737,7 +10887,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -10751,7 +10901,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -10762,23 +10912,48 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>18:52:36</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>19:57</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>65</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>18:46:03</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B46" t="inlineStr">
         <is>
           <t>19:58</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="D46" t="n">
         <v>72</v>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 995
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E332"/>
+  <dimension ref="A1:E339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:36</t>
+          <t>Última actualización: 19:12:12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 327</t>
+          <t>Total filas: 334</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,7 +5203,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5213,11 +5213,11 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6003,7 +6003,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6013,11 +6013,11 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D310" t="n">
@@ -8103,7 +8103,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -8117,7 +8117,7 @@
         </is>
       </c>
       <c r="D311" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8128,7 +8128,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
@@ -8142,7 +8142,7 @@
         </is>
       </c>
       <c r="D312" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8153,7 +8153,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -8167,7 +8167,7 @@
         </is>
       </c>
       <c r="D313" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8242,7 +8242,7 @@
         </is>
       </c>
       <c r="D316" t="n">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8278,7 +8278,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -8292,7 +8292,7 @@
         </is>
       </c>
       <c r="D318" t="n">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8303,7 +8303,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8317,7 +8317,7 @@
         </is>
       </c>
       <c r="D319" t="n">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8353,7 +8353,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -8367,7 +8367,7 @@
         </is>
       </c>
       <c r="D321" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8378,7 +8378,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -8392,7 +8392,7 @@
         </is>
       </c>
       <c r="D322" t="n">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8417,7 +8417,7 @@
         </is>
       </c>
       <c r="D323" t="n">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,12 +8428,12 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:56</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -8442,7 +8442,7 @@
         </is>
       </c>
       <c r="D324" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,12 +8453,12 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>20:05</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -8467,7 +8467,7 @@
         </is>
       </c>
       <c r="D325" t="n">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,21 +8478,21 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>18:46:03</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>20:05</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8503,21 +8503,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,12 +8528,12 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -8542,7 +8542,7 @@
         </is>
       </c>
       <c r="D328" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,21 +8553,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8578,21 +8578,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8603,12 +8603,12 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -8617,7 +8617,7 @@
         </is>
       </c>
       <c r="D331" t="n">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,23 +8628,198 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>79</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>20:33</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>81</v>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
           <t>18:52:36</t>
         </is>
       </c>
-      <c r="B332" t="inlineStr">
+      <c r="B334" t="inlineStr">
         <is>
           <t>20:47</t>
         </is>
       </c>
-      <c r="C332" t="inlineStr">
+      <c r="C334" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D332" t="n">
+      <c r="D334" t="n">
         <v>115</v>
       </c>
-      <c r="E332" t="inlineStr">
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>20:48</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>96</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>20:48</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>96</v>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>105</v>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>115</v>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>21:10</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>118</v>
+      </c>
+      <c r="E339" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8661,7 +8836,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8679,14 +8854,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:36</t>
+          <t>Última actualización: 19:12:12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 47</t>
         </is>
       </c>
     </row>
@@ -9795,7 +9970,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -9809,7 +9984,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -9820,7 +9995,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -9834,7 +10009,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -9862,6 +10037,31 @@
         <v>115</v>
       </c>
       <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>20:48</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>96</v>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9878,7 +10078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9896,14 +10096,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:36</t>
+          <t>Última actualización: 19:12:12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -10262,7 +10462,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -10272,11 +10472,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -10287,7 +10487,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -10297,11 +10497,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -10887,7 +11087,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -10901,7 +11101,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -10937,7 +11137,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -10951,9 +11151,34 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="E46" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>100</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 996
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E339"/>
+  <dimension ref="A1:E348"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:12:12</t>
+          <t>Última actualización: 19:37:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 334</t>
+          <t>Total filas: 343</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7288,11 +7288,11 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7438,7 +7438,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -7463,7 +7463,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D285" t="n">
@@ -7488,7 +7488,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8113,7 +8113,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D311" t="n">
@@ -8138,7 +8138,7 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D312" t="n">
@@ -8328,21 +8328,21 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>18:11:21</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>19:48</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8353,21 +8353,21 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>18:11:21</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:48</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8378,21 +8378,21 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,21 +8428,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>19:56</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,12 +8453,12 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:56</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -8467,7 +8467,7 @@
         </is>
       </c>
       <c r="D325" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,12 +8478,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>18:46:03</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>20:05</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -8492,7 +8492,7 @@
         </is>
       </c>
       <c r="D326" t="n">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8503,21 +8503,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>20:05</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,21 +8528,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:06</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8558,16 +8558,16 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8578,21 +8578,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8603,21 +8603,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,21 +8628,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8653,21 +8653,21 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>20:33</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,21 +8678,21 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8708,16 +8708,16 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>20:48</t>
+          <t>20:33</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8728,21 +8728,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>20:48</t>
+          <t>20:34</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8753,21 +8753,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8778,21 +8778,21 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8808,18 +8808,243 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
+          <t>20:48</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>96</v>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>20:48</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>96</v>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>19:37:39</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>20:53</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>76</v>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>19:37:39</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>20:55</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>78</v>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>105</v>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>19:37:39</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>21:06</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>89</v>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>19:12:11</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>115</v>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>19:37:39</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
           <t>21:10</t>
         </is>
       </c>
-      <c r="C339" t="inlineStr">
+      <c r="C346" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D339" t="n">
-        <v>118</v>
-      </c>
-      <c r="E339" t="inlineStr">
+      <c r="D346" t="n">
+        <v>93</v>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>19:37:39</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>111</v>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>19:37:39</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>117</v>
+      </c>
+      <c r="E348" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8836,7 +9061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8854,14 +9079,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:12:12</t>
+          <t>Última actualización: 19:37:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 47</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -9995,12 +10220,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>20:06</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -10009,7 +10234,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -10020,21 +10245,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>115</v>
+        <v>55</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -10045,23 +10270,48 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>19:37:39</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>20:47</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>70</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
           <t>19:12:11</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B53" t="inlineStr">
         <is>
           <t>20:48</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D52" t="n">
+      <c r="D53" t="n">
         <v>96</v>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10078,7 +10328,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10096,14 +10346,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:12:12</t>
+          <t>Última actualización: 19:37:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 43</t>
         </is>
       </c>
     </row>
@@ -11112,7 +11362,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -11126,7 +11376,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -11162,23 +11412,48 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>19:37:39</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>20:51</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>74</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>19:12:11</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>20:52</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="D48" t="n">
         <v>100</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 997
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E348"/>
+  <dimension ref="A1:E352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:37:39</t>
+          <t>Última actualización: 19:50:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 343</t>
+          <t>Total filas: 347</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6003,7 +6003,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6013,11 +6013,11 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7288,11 +7288,11 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7438,7 +7438,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -7463,7 +7463,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D285" t="n">
@@ -7488,7 +7488,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8378,7 +8378,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -8392,7 +8392,7 @@
         </is>
       </c>
       <c r="D322" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8438,7 +8438,7 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D324" t="n">
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8567,7 +8567,7 @@
         </is>
       </c>
       <c r="D329" t="n">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8578,21 +8578,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8603,12 +8603,12 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -8617,7 +8617,7 @@
         </is>
       </c>
       <c r="D331" t="n">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,21 +8628,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8653,21 +8653,21 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,12 +8678,12 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
@@ -8692,7 +8692,7 @@
         </is>
       </c>
       <c r="D334" t="n">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8708,16 +8708,16 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>20:33</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8728,12 +8728,12 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>20:34</t>
+          <t>20:33</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
@@ -8742,7 +8742,7 @@
         </is>
       </c>
       <c r="D336" t="n">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8753,21 +8753,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>20:45</t>
+          <t>20:34</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8783,16 +8783,16 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8803,21 +8803,21 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>20:48</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8828,21 +8828,21 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>20:48</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8853,21 +8853,21 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>20:48</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8878,21 +8878,21 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:48</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8903,12 +8903,12 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
@@ -8917,7 +8917,7 @@
         </is>
       </c>
       <c r="D343" t="n">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8928,21 +8928,21 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8953,21 +8953,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8978,21 +8978,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:06</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9003,21 +9003,21 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,23 +9028,123 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
+          <t>21:10</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>80</v>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>19:50:34</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>98</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>19:50:34</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>100</v>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>19:50:34</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
           <t>21:34</t>
         </is>
       </c>
-      <c r="C348" t="inlineStr">
+      <c r="C351" t="inlineStr">
         <is>
           <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
-      <c r="D348" t="n">
-        <v>117</v>
-      </c>
-      <c r="E348" t="inlineStr">
+      <c r="D351" t="n">
+        <v>104</v>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>19:50:34</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>116</v>
+      </c>
+      <c r="E352" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9079,7 +9179,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:37:39</t>
+          <t>Última actualización: 19:50:34</t>
         </is>
       </c>
     </row>
@@ -10245,7 +10345,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -10259,7 +10359,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -10270,7 +10370,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -10284,7 +10384,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -10328,7 +10428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10346,14 +10446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:37:39</t>
+          <t>Última actualización: 19:50:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 43</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -10712,7 +10812,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -10722,11 +10822,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -10737,7 +10837,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -10747,11 +10847,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -11412,7 +11512,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -11426,7 +11526,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -11454,6 +11554,31 @@
         <v>100</v>
       </c>
       <c r="E48" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>19:50:34</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>21:27</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>97</v>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 998
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E352"/>
+  <dimension ref="A1:E355"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:50:34</t>
+          <t>Última actualización: 20:12:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 347</t>
+          <t>Total filas: 350</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6003,7 +6003,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6013,11 +6013,11 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7438,7 +7438,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8603,7 +8603,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8617,7 +8617,7 @@
         </is>
       </c>
       <c r="D331" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8703,7 +8703,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
@@ -8717,7 +8717,7 @@
         </is>
       </c>
       <c r="D335" t="n">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8753,7 +8753,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -8767,7 +8767,7 @@
         </is>
       </c>
       <c r="D337" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8803,7 +8803,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
@@ -8817,7 +8817,7 @@
         </is>
       </c>
       <c r="D339" t="n">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8828,7 +8828,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -8842,7 +8842,7 @@
         </is>
       </c>
       <c r="D340" t="n">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8863,7 +8863,7 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D341" t="n">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8928,7 +8928,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
@@ -8942,7 +8942,7 @@
         </is>
       </c>
       <c r="D344" t="n">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8953,7 +8953,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
@@ -8967,7 +8967,7 @@
         </is>
       </c>
       <c r="D345" t="n">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -9003,7 +9003,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -9017,7 +9017,7 @@
         </is>
       </c>
       <c r="D347" t="n">
-        <v>115</v>
+        <v>55</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,7 +9028,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -9042,7 +9042,7 @@
         </is>
       </c>
       <c r="D348" t="n">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,7 +9053,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
@@ -9067,7 +9067,7 @@
         </is>
       </c>
       <c r="D349" t="n">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9103,21 +9103,21 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:31</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9128,23 +9128,98 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>82</v>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>20:12:18</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>21:45</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D353" t="n">
+        <v>93</v>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>20:12:18</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
           <t>21:46</t>
         </is>
       </c>
-      <c r="C352" t="inlineStr">
+      <c r="C354" t="inlineStr">
         <is>
           <t>14X44_ABASTO</t>
         </is>
       </c>
-      <c r="D352" t="n">
-        <v>116</v>
-      </c>
-      <c r="E352" t="inlineStr">
+      <c r="D354" t="n">
+        <v>94</v>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>20:12:18</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>112</v>
+      </c>
+      <c r="E355" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9179,7 +9254,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:50:34</t>
+          <t>Última actualización: 20:12:18</t>
         </is>
       </c>
     </row>
@@ -10370,7 +10445,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -10384,7 +10459,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -10428,7 +10503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10446,14 +10521,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:50:34</t>
+          <t>Última actualización: 20:12:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -11537,7 +11612,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -11551,7 +11626,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -11579,6 +11654,31 @@
         <v>97</v>
       </c>
       <c r="E49" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>20:12:18</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>78</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 999
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E355"/>
+  <dimension ref="A1:E360"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:12:18</t>
+          <t>Última actualización: 20:33:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 350</t>
+          <t>Total filas: 355</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4713,11 +4713,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D224" t="n">
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6003,7 +6003,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6013,11 +6013,11 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7288,11 +7288,11 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7463,7 +7463,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D285" t="n">
@@ -7488,7 +7488,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8563,7 +8563,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D329" t="n">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D330" t="n">
@@ -8753,7 +8753,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -8767,7 +8767,7 @@
         </is>
       </c>
       <c r="D337" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8803,7 +8803,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
@@ -8817,7 +8817,7 @@
         </is>
       </c>
       <c r="D339" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8828,7 +8828,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -8842,7 +8842,7 @@
         </is>
       </c>
       <c r="D340" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8863,7 +8863,7 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D341" t="n">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8978,21 +8978,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9003,21 +9003,21 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>21:05</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,21 +9028,21 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:06</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,21 +9053,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,21 +9078,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9103,21 +9103,21 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>21:31</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9128,21 +9128,21 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:30</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9158,16 +9158,16 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>21:31</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9178,21 +9178,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9203,23 +9203,148 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
+          <t>20:33:22</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>61</v>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
           <t>20:12:18</t>
         </is>
       </c>
-      <c r="B355" t="inlineStr">
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>21:45</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>93</v>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>20:33:22</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
+        <v>73</v>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>20:33:22</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>73</v>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>20:33:22</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
         <is>
           <t>22:04</t>
         </is>
       </c>
-      <c r="C355" t="inlineStr">
+      <c r="C359" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D355" t="n">
-        <v>112</v>
-      </c>
-      <c r="E355" t="inlineStr">
+      <c r="D359" t="n">
+        <v>91</v>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>20:33:22</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>22:11</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D360" t="n">
+        <v>98</v>
+      </c>
+      <c r="E360" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9254,7 +9379,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:12:18</t>
+          <t>Última actualización: 20:33:22</t>
         </is>
       </c>
     </row>
@@ -10445,7 +10570,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -10459,7 +10584,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -10503,7 +10628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10521,14 +10646,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:12:18</t>
+          <t>Última actualización: 20:33:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
     </row>
@@ -11612,7 +11737,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -11626,7 +11751,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -11681,6 +11806,31 @@
       <c r="E50" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>20:33:22</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>107</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1000
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E360"/>
+  <dimension ref="A1:E365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:33:22</t>
+          <t>Última actualización: 20:47:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 355</t>
+          <t>Total filas: 360</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,7 +5203,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5213,11 +5213,11 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>14:53:58</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D224" t="n">
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:53:58</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6003,7 +6003,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6013,11 +6013,11 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8113,7 +8113,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D311" t="n">
@@ -8138,7 +8138,7 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D312" t="n">
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8563,7 +8563,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D329" t="n">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D330" t="n">
@@ -8828,7 +8828,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -8842,7 +8842,7 @@
         </is>
       </c>
       <c r="D340" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8853,7 +8853,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -8863,11 +8863,11 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -9003,12 +9003,12 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>21:05</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
@@ -9017,7 +9017,7 @@
         </is>
       </c>
       <c r="D347" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,21 +9028,21 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>21:05</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,12 +9053,12 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>21:06</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
@@ -9067,7 +9067,7 @@
         </is>
       </c>
       <c r="D349" t="n">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,21 +9078,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9103,21 +9103,21 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9128,21 +9128,21 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>21:11</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9153,21 +9153,21 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>21:31</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9178,21 +9178,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:30</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9203,12 +9203,12 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:31</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
@@ -9217,7 +9217,7 @@
         </is>
       </c>
       <c r="D355" t="n">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9228,21 +9228,21 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9253,21 +9253,21 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D357" t="n">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9278,12 +9278,12 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
@@ -9292,7 +9292,7 @@
         </is>
       </c>
       <c r="D358" t="n">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9308,16 +9308,16 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9328,23 +9328,148 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
         <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D360" t="n">
+        <v>59</v>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>20:47:15</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>77</v>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>20:47:15</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
           <t>22:11</t>
         </is>
       </c>
-      <c r="C360" t="inlineStr">
+      <c r="C362" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D360" t="n">
-        <v>98</v>
-      </c>
-      <c r="E360" t="inlineStr">
+      <c r="D362" t="n">
+        <v>84</v>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>20:47:15</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>107</v>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>20:47:15</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>107</v>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>20:47:15</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>22:44</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>117</v>
+      </c>
+      <c r="E365" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9361,7 +9486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9379,14 +9504,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:33:22</t>
+          <t>Última actualización: 20:47:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 48</t>
+          <t>Total filas: 49</t>
         </is>
       </c>
     </row>
@@ -10570,7 +10695,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -10584,7 +10709,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -10612,6 +10737,31 @@
         <v>96</v>
       </c>
       <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>20:47:15</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>107</v>
+      </c>
+      <c r="E54" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10628,7 +10778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10646,14 +10796,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:33:22</t>
+          <t>Última actualización: 20:47:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 47</t>
         </is>
       </c>
     </row>
@@ -11762,12 +11912,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>21:27</t>
+          <t>20:54</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -11776,7 +11926,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -11787,12 +11937,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>21:27</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -11801,7 +11951,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -11812,23 +11962,48 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>43</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>20:47:15</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>22:20</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D51" t="n">
-        <v>107</v>
-      </c>
-      <c r="E51" t="inlineStr">
+      <c r="D52" t="n">
+        <v>93</v>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1001
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E365"/>
+  <dimension ref="A1:E369"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:47:15</t>
+          <t>Última actualización: 20:54:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 360</t>
+          <t>Total filas: 364</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1363,11 +1363,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>07:52:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:52:32</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3528,7 +3528,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3538,11 +3538,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,7 +3553,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>12:54:41</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4438,11 +4438,11 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:54:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:43:25</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:43:25</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>14:15:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,7 +5203,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>14:15:21</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -5213,11 +5213,11 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:47:05</t>
+          <t>15:47:47</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:47:47</t>
+          <t>14:47:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:52:32</t>
+          <t>16:44:07</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>16:44:07</t>
+          <t>16:52:32</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7288,11 +7288,11 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7438,7 +7438,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8853,7 +8853,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -8863,11 +8863,11 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8878,7 +8878,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -8888,11 +8888,11 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8953,7 +8953,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
@@ -8963,11 +8963,11 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8978,7 +8978,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -8988,11 +8988,11 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9003,12 +9003,12 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
@@ -9017,7 +9017,7 @@
         </is>
       </c>
       <c r="D347" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,12 +9028,12 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>21:05</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
@@ -9042,7 +9042,7 @@
         </is>
       </c>
       <c r="D348" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,21 +9053,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>21:05</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,12 +9078,12 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>21:06</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
@@ -9092,7 +9092,7 @@
         </is>
       </c>
       <c r="D350" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9108,16 +9108,16 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9128,21 +9128,21 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>21:11</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9158,16 +9158,16 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>21:11</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9178,21 +9178,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>21:18</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9203,21 +9203,21 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>21:31</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9228,21 +9228,21 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:30</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9253,12 +9253,12 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:31</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
@@ -9267,7 +9267,7 @@
         </is>
       </c>
       <c r="D357" t="n">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9278,21 +9278,21 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9303,21 +9303,21 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9328,21 +9328,21 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9353,21 +9353,21 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D361" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9378,21 +9378,21 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>22:11</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D362" t="n">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -9403,21 +9403,21 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>22:34</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D363" t="n">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -9428,21 +9428,21 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>22:34</t>
+          <t>22:11</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9453,23 +9453,123 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
+          <t>20:54:27</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>22:33</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>99</v>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
           <t>20:47:15</t>
         </is>
       </c>
-      <c r="B365" t="inlineStr">
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>107</v>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>20:54:27</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D367" t="n">
+        <v>100</v>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>20:54:27</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>22:43</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D368" t="n">
+        <v>109</v>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>20:47:15</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
         <is>
           <t>22:44</t>
         </is>
       </c>
-      <c r="C365" t="inlineStr">
+      <c r="C369" t="inlineStr">
         <is>
           <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D365" t="n">
+      <c r="D369" t="n">
         <v>117</v>
       </c>
-      <c r="E365" t="inlineStr">
+      <c r="E369" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9486,7 +9586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9504,14 +9604,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:47:15</t>
+          <t>Última actualización: 20:54:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 49</t>
+          <t>Total filas: 50</t>
         </is>
       </c>
     </row>
@@ -10745,23 +10845,48 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>20:54:27</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>22:33</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>99</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>20:47:15</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B55" t="inlineStr">
         <is>
           <t>22:34</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D54" t="n">
+      <c r="D55" t="n">
         <v>107</v>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10778,7 +10903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10796,14 +10921,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:47:15</t>
+          <t>Última actualización: 20:54:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 47</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -11162,7 +11287,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -11172,11 +11297,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -11187,7 +11312,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -11197,11 +11322,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -11937,12 +12062,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>21:27</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -11951,7 +12076,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -11962,12 +12087,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>21:27</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -11976,7 +12101,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -11987,23 +12112,48 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>36</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>20:54:27</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
           <t>22:20</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D52" t="n">
-        <v>93</v>
-      </c>
-      <c r="E52" t="inlineStr">
+      <c r="D53" t="n">
+        <v>86</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1002
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-25.xlsx
+++ b/data/horarios-141-2026-01-25.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E369"/>
+  <dimension ref="A1:E377"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:54:27</t>
+          <t>Última actualización: 22:05:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 364</t>
+          <t>Total filas: 372</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:38:54</t>
+          <t>05:44:02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -738,11 +738,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:44:02</t>
+          <t>06:38:54</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -763,11 +763,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>07:15:48</t>
+          <t>06:56:24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:56:24</t>
+          <t>07:15:48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1063,11 +1063,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:40:59</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:40:59</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:52:33</t>
+          <t>08:30:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:30:14</t>
+          <t>08:52:33</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:56:01</t>
+          <t>09:23:52</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:23:52</t>
+          <t>10:56:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:07:51</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>10:07:51</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:48:20</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:48:20</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3713,11 +3713,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4003,7 +4003,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>11:35:40</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:35:40</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:13:01</t>
+          <t>12:33:54</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:33:54</t>
+          <t>11:13:01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:55:01</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4338,11 +4338,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>11:55:01</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4728,7 +4728,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>12:47:00</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4738,11 +4738,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:47:00</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:57:31</t>
+          <t>13:14:41</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4988,11 +4988,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:14:41</t>
+          <t>13:57:31</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5913,7 +5913,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D223" t="n">
@@ -5938,7 +5938,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D224" t="n">
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>15:17:56</t>
+          <t>14:33:43</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:33:43</t>
+          <t>15:17:56</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5988,11 +5988,11 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7288,11 +7288,11 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7438,7 +7438,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D284" t="n">
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:38:13</t>
+          <t>17:51:15</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:51:15</t>
+          <t>17:38:13</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>18:52:36</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>18:52:36</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>19:37:39</t>
+          <t>19:50:34</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>19:50:34</t>
+          <t>19:37:39</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8853,7 +8853,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>19:12:11</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -8863,11 +8863,11 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8878,7 +8878,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>19:12:11</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -8888,11 +8888,11 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8953,7 +8953,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:12:18</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
@@ -8963,11 +8963,11 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8978,7 +8978,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>20:12:18</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -8988,11 +8988,11 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9288,7 +9288,7 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D358" t="n">
@@ -9313,7 +9313,7 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D359" t="n">
@@ -9353,7 +9353,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>20:54:27</t>
+          <t>20:33:22</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
@@ -9363,11 +9363,11 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D361" t="n">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9378,7 +9378,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>20:33:22</t>
+          <t>20:54:27</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
@@ -9388,11 +9388,11 @@
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D362" t="n">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -9428,21 +9428,21 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>20:54:27</t>
+          <t>22:05:43</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>22:11</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9453,21 +9453,21 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>20:54:27</t>
+          <t>22:05:43</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>22:33</t>
+          <t>22:11</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9478,21 +9478,21 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>20:47:15</t>
+          <t>22:05:43</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>22:34</t>
+          <t>22:29</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9503,21 +9503,21 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>20:54:27</t>
+          <t>22:05:43</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>22:34</t>
+          <t>22:33</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9528,21 +9528,21 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>20:54:27</t>
+          <t>20:47:15</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>22:43</t>
+          <t>22:34</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D368" t="n">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -9553,23 +9553,223 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
+          <t>22:05:43</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>29</v>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>22:05:43</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>22:43</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D370" t="n">
+        <v>38</v>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
           <t>20:47:15</t>
         </is>
       </c>
-      <c r="B369" t="inlineStr">
+      <c r="B371" t="inlineStr">
         <is>
           <t>22:44</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
+      <c r="C371" t="inlineStr">
         <is>
           <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D369" t="n">
+      <c r="D371" t="n">
         <v>117</v>
       </c>
-      <c r="E369" t="inlineStr">
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>22:05:43</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>23:04</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D372" t="n">
+        <v>59</v>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>22:05:43</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>23:19</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D373" t="n">
+        <v>74</v>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>22:05:43</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>23:34</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D374" t="n">
+        <v>89</v>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>22:05:43</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>23:39</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D375" t="n">
+        <v>94</v>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>22:05:43</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>23:40</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D376" t="n">
+        <v>95</v>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>22:05:43</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>23:58</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D377" t="n">
+        <v>113</v>
+      </c>
+      <c r="E377" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9586,7 +9786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9604,14 +9804,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:54:27</t>
+          <t>Última actualización: 22:05:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 50</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
     </row>
@@ -10845,7 +11045,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20:54:27</t>
+          <t>22:05:43</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -10859,7 +11059,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>99</v>
+        <v>28</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -10887,6 +11087,31 @@
         <v>107</v>
       </c>
       <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>22:05:43</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>23:39</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>94</v>
+      </c>
+      <c r="E56" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10903,7 +11128,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10921,14 +11146,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:54:27</t>
+          <t>Última actualización: 22:05:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 48</t>
+          <t>Total filas: 49</t>
         </is>
       </c>
     </row>
@@ -12137,23 +12362,48 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>22:05:43</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>22:19</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>14</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>20:54:27</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B54" t="inlineStr">
         <is>
           <t>22:20</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D53" t="n">
+      <c r="D54" t="n">
         <v>86</v>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>